<commit_message>
Updated with new concept
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GREENLAND\JulieFiling\Filing\Canada Health Infoway\Dosage Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Filing\Canada Health Infoway\GitHub\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="417">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -812,9 +812,6 @@
   </si>
   <si>
     <t>Semi-solid preparation consisting of a gel usually presented in a single-dose container provided with a suitable applicator, intended for rectal use to obtain a local effect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not currently present in EDQM but uses EDQM pattern.  Likely to be a patient-friendly term rather than a full dose form concept </t>
   </si>
   <si>
     <t>rectal liquid</t>
@@ -1288,6 +1285,131 @@
   </si>
   <si>
     <t>suppositoire</t>
+  </si>
+  <si>
+    <t>Used as a placeholder; correct dose forms are added to concepts using the Combination product table</t>
+  </si>
+  <si>
+    <t>anticoagulant and preservative solution for blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liquid sterile preparation consisting of an aqueous solution to be mixed with extracorporeal blood</t>
+  </si>
+  <si>
+    <t>solution anticoagulante et de conservation du sang humain</t>
+  </si>
+  <si>
+    <t>comprimé sublingual</t>
+  </si>
+  <si>
+    <t>solution pour pulvérisation sublinguale</t>
+  </si>
+  <si>
+    <t>solution pour dialyse péritonéale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solution injectable </t>
+  </si>
+  <si>
+    <t>solution pour hémodialyse</t>
+  </si>
+  <si>
+    <t>solution de cardioplégie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shampoing </t>
+  </si>
+  <si>
+    <t>suspension rectale</t>
+  </si>
+  <si>
+    <t>solution rectale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pommade rectale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+gel rectal </t>
+  </si>
+  <si>
+    <t>Not EDQM but uses EDQM pattern</t>
+  </si>
+  <si>
+    <t>liquide oral</t>
+  </si>
+  <si>
+    <t>liquide rectale</t>
+  </si>
+  <si>
+    <t>mousse rectale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crème rectale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+suspension injectable à libération prolongée</t>
+  </si>
+  <si>
+    <t>poudre péridontale à libération prolongée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collyre à libération prolongée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">comprimé oral à libération prolongée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">capsule oral à libération prolongée </t>
+  </si>
+  <si>
+    <t>inhalation en flacon pressurisé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre pour suspension injectable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre pour solution injectable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre pour suspension injectable pour perfusion </t>
+  </si>
+  <si>
+    <t>poudre pour suspension injectable à libération prolongée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre pour solution rectale </t>
+  </si>
+  <si>
+    <t>poudre pour suspension oral/rectal</t>
+  </si>
+  <si>
+    <t>poudre pour inhalation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre pour inhalation en gélule </t>
+  </si>
+  <si>
+    <t>solution à inhaler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liquide pour inhalation par vapeur </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gel intestinal </t>
+  </si>
+  <si>
+    <t>système de diffusion intra-utérin</t>
+  </si>
+  <si>
+    <t>solution intravésicale</t>
+  </si>
+  <si>
+    <t>implant vitréen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solution pour irrigation </t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1469,6 +1591,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,24 +1880,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="120.28515625" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.5703125" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1777,8 +1908,8 @@
       <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>325</v>
+      <c r="E1" s="28" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1792,8 +1923,8 @@
         <v>4</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" t="s">
-        <v>326</v>
+      <c r="E2" s="29" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1801,13 +1932,13 @@
         <v>40146</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>327</v>
+        <v>312</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1823,8 +1954,8 @@
       <c r="D4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>328</v>
+      <c r="E4" s="29" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1840,8 +1971,8 @@
       <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>330</v>
+      <c r="E5" s="29" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1855,8 +1986,8 @@
         <v>12</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" t="s">
-        <v>329</v>
+      <c r="E6" s="29" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1870,8 +2001,8 @@
         <v>14</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="12" t="s">
-        <v>331</v>
+      <c r="E7" s="30" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1885,10 +2016,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="E8" t="s">
-        <v>335</v>
+        <v>331</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1904,8 +2035,8 @@
       <c r="D9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>334</v>
+      <c r="E9" s="30" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1921,8 +2052,8 @@
       <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>336</v>
+      <c r="E10" s="30" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1936,8 +2067,8 @@
         <v>24</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="12" t="s">
-        <v>337</v>
+      <c r="E11" s="30" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1951,8 +2082,8 @@
         <v>26</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="12" t="s">
-        <v>338</v>
+      <c r="E12" s="30" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,11 +2097,11 @@
         <v>28</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="12" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>40124</v>
       </c>
@@ -1981,8 +2112,8 @@
         <v>30</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="12" t="s">
-        <v>340</v>
+      <c r="E14" s="30" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1998,8 +2129,8 @@
       <c r="D15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>341</v>
+      <c r="E15" s="30" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2013,8 +2144,8 @@
         <v>35</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="12" t="s">
-        <v>342</v>
+      <c r="E16" s="30" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2028,8 +2159,8 @@
         <v>37</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="12" t="s">
-        <v>343</v>
+      <c r="E17" s="30" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2043,8 +2174,8 @@
         <v>39</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="12" t="s">
-        <v>344</v>
+      <c r="E18" s="30" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,8 +2189,8 @@
         <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="12" t="s">
-        <v>345</v>
+      <c r="E19" s="30" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2075,8 +2206,8 @@
       <c r="D20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>354</v>
+      <c r="E20" s="30" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2087,11 +2218,11 @@
         <v>44</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D21" s="27"/>
-      <c r="E21" s="25" t="s">
-        <v>346</v>
+      <c r="E21" s="31" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2107,8 +2238,8 @@
       <c r="D22" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>353</v>
+      <c r="E22" s="30" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2122,8 +2253,8 @@
         <v>48</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="12" t="s">
-        <v>348</v>
+      <c r="E23" s="30" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2137,8 +2268,8 @@
         <v>50</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="12" t="s">
-        <v>355</v>
+      <c r="E24" s="30" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2152,8 +2283,8 @@
         <v>52</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="12" t="s">
-        <v>356</v>
+      <c r="E25" s="30" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2169,8 +2300,8 @@
       <c r="D26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>357</v>
+      <c r="E26" s="30" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2184,8 +2315,8 @@
         <v>57</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="12" t="s">
-        <v>358</v>
+      <c r="E27" s="30" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2201,8 +2332,8 @@
       <c r="D28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>359</v>
+      <c r="E28" s="30" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2216,8 +2347,8 @@
         <v>62</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="12" t="s">
-        <v>360</v>
+      <c r="E29" s="30" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2233,8 +2364,8 @@
       <c r="D30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>361</v>
+      <c r="E30" s="30" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2248,8 +2379,8 @@
         <v>66</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" t="s">
-        <v>349</v>
+      <c r="E31" s="29" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2263,11 +2394,11 @@
         <v>68</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="12" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E32" s="30" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>40101</v>
       </c>
@@ -2278,8 +2409,11 @@
         <v>70</v>
       </c>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E33" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>40025</v>
       </c>
@@ -2290,8 +2424,11 @@
         <v>72</v>
       </c>
       <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E34" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>40022</v>
       </c>
@@ -2302,8 +2439,11 @@
         <v>74</v>
       </c>
       <c r="D35" s="15"/>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" s="29" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>40027</v>
       </c>
@@ -2314,8 +2454,11 @@
         <v>76</v>
       </c>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E36" s="29" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>40024</v>
       </c>
@@ -2326,8 +2469,11 @@
         <v>78</v>
       </c>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="29" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>40034</v>
       </c>
@@ -2338,8 +2484,11 @@
         <v>80</v>
       </c>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="30" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>40038</v>
       </c>
@@ -2350,8 +2499,11 @@
         <v>82</v>
       </c>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>40041</v>
       </c>
@@ -2362,8 +2514,11 @@
         <v>84</v>
       </c>
       <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E40" s="30" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>40042</v>
       </c>
@@ -2376,8 +2531,11 @@
       <c r="D41" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E41" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>40035</v>
       </c>
@@ -2388,17 +2546,23 @@
         <v>89</v>
       </c>
       <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="E42" s="29" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23">
         <v>40006</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="C43" s="12"/>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="E43" s="29"/>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>40115</v>
       </c>
@@ -2409,10 +2573,10 @@
         <v>91</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <v>40114</v>
       </c>
@@ -2423,10 +2587,10 @@
         <v>93</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>40073</v>
       </c>
@@ -2438,7 +2602,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>40130</v>
       </c>
@@ -2450,7 +2614,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>40023</v>
       </c>
@@ -2463,13 +2627,14 @@
       <c r="D48" s="12" t="s">
         <v>100</v>
       </c>
+      <c r="E48" s="29"/>
     </row>
     <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>40061</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>101</v>
@@ -2483,7 +2648,7 @@
         <v>40080</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>103</v>
@@ -2658,7 +2823,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>40052</v>
       </c>
@@ -2701,28 +2866,30 @@
         <v>40058</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>289</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="E67" s="29"/>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>40059</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>291</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="E68" s="29"/>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
@@ -2746,7 +2913,7 @@
         <v>145</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>146</v>
@@ -2757,14 +2924,14 @@
         <v>40144</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D71" s="12"/>
-      <c r="E71" s="17" t="s">
-        <v>351</v>
+      <c r="E71" s="29" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2772,12 +2939,13 @@
         <v>40145</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D72" s="12"/>
+      <c r="E72" s="29"/>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
@@ -2802,8 +2970,8 @@
         <v>150</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" t="s">
-        <v>352</v>
+      <c r="E74" s="29" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2817,6 +2985,9 @@
         <v>152</v>
       </c>
       <c r="D75" s="1"/>
+      <c r="E75" s="29" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
@@ -2880,7 +3051,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>40066</v>
       </c>
@@ -2892,7 +3063,7 @@
       </c>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>40076</v>
       </c>
@@ -2904,7 +3075,7 @@
       </c>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>40002</v>
       </c>
@@ -2916,7 +3087,7 @@
       </c>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>40009</v>
       </c>
@@ -2928,18 +3099,19 @@
       </c>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>40008</v>
       </c>
       <c r="B85" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C85" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="C85" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E85" s="29"/>
+    </row>
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>40005</v>
       </c>
@@ -2953,7 +3125,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>40089</v>
       </c>
@@ -2967,7 +3139,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>40086</v>
       </c>
@@ -2981,7 +3153,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>40087</v>
       </c>
@@ -2995,7 +3167,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>40088</v>
       </c>
@@ -3009,7 +3181,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>40090</v>
       </c>
@@ -3023,21 +3195,22 @@
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>40117</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C92" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D92" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="D92" s="17" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="29"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>40102</v>
       </c>
@@ -3049,7 +3222,7 @@
       </c>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>40139</v>
       </c>
@@ -3061,21 +3234,22 @@
       </c>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>40120</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C95" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D95" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="D95" s="17" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E95" s="29"/>
+    </row>
+    <row r="96" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>40014</v>
       </c>
@@ -3087,7 +3261,7 @@
       </c>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>40122</v>
       </c>
@@ -3099,7 +3273,7 @@
       </c>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>40040</v>
       </c>
@@ -3111,7 +3285,7 @@
       </c>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>40026</v>
       </c>
@@ -3123,7 +3297,7 @@
       </c>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>40054</v>
       </c>
@@ -3137,7 +3311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>40049</v>
       </c>
@@ -3145,21 +3319,21 @@
         <v>205</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="22"/>
       <c r="B102" s="4" t="s">
         <v>206</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>40085</v>
       </c>
@@ -3170,8 +3344,11 @@
         <v>208</v>
       </c>
       <c r="D103" s="1"/>
-    </row>
-    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E103" s="29" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>40018</v>
       </c>
@@ -3182,8 +3359,11 @@
         <v>210</v>
       </c>
       <c r="D104" s="1"/>
-    </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E104" s="29" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>40096</v>
       </c>
@@ -3194,8 +3374,11 @@
         <v>212</v>
       </c>
       <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E105" s="29" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>40017</v>
       </c>
@@ -3206,8 +3389,11 @@
         <v>214</v>
       </c>
       <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E106" s="29" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>40039</v>
       </c>
@@ -3220,8 +3406,11 @@
       <c r="D107" s="12" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E107" s="29" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>40016</v>
       </c>
@@ -3232,8 +3421,11 @@
         <v>219</v>
       </c>
       <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E108" s="29" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>40021</v>
       </c>
@@ -3244,44 +3436,56 @@
         <v>221</v>
       </c>
       <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E109" s="29" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>40055</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C110" s="12" t="s">
         <v>222</v>
       </c>
       <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E110" s="29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>40062</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>223</v>
       </c>
       <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E111" s="29" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>40083</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>224</v>
       </c>
       <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E112" s="29" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>40103</v>
       </c>
@@ -3294,8 +3498,11 @@
       <c r="D113" s="6" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E113" s="30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>40020</v>
       </c>
@@ -3306,8 +3513,11 @@
         <v>229</v>
       </c>
       <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E114" s="30" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>40099</v>
       </c>
@@ -3318,8 +3528,11 @@
         <v>231</v>
       </c>
       <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E115" s="29" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>40091</v>
       </c>
@@ -3330,8 +3543,11 @@
         <v>233</v>
       </c>
       <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E116" s="30" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>40093</v>
       </c>
@@ -3341,139 +3557,174 @@
       <c r="C117" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="D117" s="12" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="12"/>
+      <c r="E117" s="30" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>40092</v>
       </c>
       <c r="B118" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C118" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="C118" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D118" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E118" s="29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>40095</v>
       </c>
       <c r="B119" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C119" s="12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E119" s="29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>40094</v>
       </c>
       <c r="B120" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C120" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C120" s="12" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E120" s="30" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>40098</v>
       </c>
       <c r="B121" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C121" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E121" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="23">
         <v>40140</v>
       </c>
       <c r="B122" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C122" s="25" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="E122" s="29"/>
+    </row>
+    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>40123</v>
       </c>
       <c r="B123" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C123" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="C123" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E123" s="29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
         <v>40032</v>
       </c>
       <c r="B124" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C124" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="C124" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E124" s="29" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
         <v>40013</v>
       </c>
       <c r="B125" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C125" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
         <v>40001</v>
       </c>
       <c r="B126" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C126" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="C126" s="12" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E126" s="29" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>40036</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C127" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="C127" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E127" s="29" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>40125</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C128" s="12"/>
+      <c r="E128" s="29"/>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
         <v>40104</v>
       </c>
       <c r="B129" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C129" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>256</v>
+      <c r="E129" s="29" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3481,10 +3732,13 @@
         <v>40105</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C130" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="C130" s="12" t="s">
-        <v>258</v>
+      <c r="E130" s="29" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3492,13 +3746,13 @@
         <v>40097</v>
       </c>
       <c r="B131" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C131" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="C131" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="E131" t="s">
-        <v>376</v>
+      <c r="E131" s="29" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3506,13 +3760,13 @@
         <v>40019</v>
       </c>
       <c r="B132" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C132" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="C132" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="E132" t="s">
-        <v>375</v>
+      <c r="E132" s="29" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3520,30 +3774,31 @@
         <v>40128</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D133" s="17" t="s">
-        <v>317</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="E133" s="29"/>
     </row>
     <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="23">
         <v>40077</v>
       </c>
       <c r="B134" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="C134" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="C134" s="25" t="s">
-        <v>264</v>
-      </c>
       <c r="D134" s="23" t="s">
-        <v>374</v>
-      </c>
-      <c r="E134" s="23" t="s">
         <v>373</v>
+      </c>
+      <c r="E134" s="32" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="135" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3551,13 +3806,13 @@
         <v>40100</v>
       </c>
       <c r="B135" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C135" s="12" t="s">
         <v>311</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="E135" s="17" t="s">
-        <v>372</v>
+      <c r="E135" s="29" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3565,13 +3820,13 @@
         <v>40012</v>
       </c>
       <c r="B136" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C136" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="C136" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="E136" t="s">
-        <v>371</v>
+      <c r="E136" s="29" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3579,27 +3834,27 @@
         <v>40132</v>
       </c>
       <c r="B137" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C137" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="C137" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="E137" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="E137" s="29" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
         <v>40133</v>
       </c>
       <c r="B138" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="C138" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="E138" t="s">
-        <v>369</v>
+      <c r="E138" s="29" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3607,13 +3862,13 @@
         <v>40135</v>
       </c>
       <c r="B139" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C139" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="E139" t="s">
-        <v>368</v>
+      <c r="E139" s="29" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3621,13 +3876,13 @@
         <v>40134</v>
       </c>
       <c r="B140" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C140" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="E140" t="s">
-        <v>367</v>
+      <c r="E140" s="29" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3635,13 +3890,13 @@
         <v>40131</v>
       </c>
       <c r="B141" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C141" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="C141" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="E141" t="s">
-        <v>366</v>
+      <c r="E141" s="29" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3649,13 +3904,13 @@
         <v>40137</v>
       </c>
       <c r="B142" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C142" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="C142" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="E142" s="12" t="s">
-        <v>365</v>
+      <c r="E142" s="30" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3663,13 +3918,13 @@
         <v>40136</v>
       </c>
       <c r="B143" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C143" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="C143" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="E143" t="s">
-        <v>364</v>
+      <c r="E143" s="29" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3677,13 +3932,13 @@
         <v>40138</v>
       </c>
       <c r="B144" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C144" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="C144" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="E144" t="s">
-        <v>362</v>
+      <c r="E144" s="29" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3691,13 +3946,13 @@
         <v>40141</v>
       </c>
       <c r="B145" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C145" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="C145" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="E145" s="12" t="s">
-        <v>363</v>
+      <c r="E145" s="30" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3705,18 +3960,29 @@
         <v>40129</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D146" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B147" s="5"/>
       <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C148" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="E148" s="29" t="s">
+        <v>379</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded revised NTP Dosage Form Concepts
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Filing\Canada Health Infoway\GitHub\formulary\Working QA Team Folders\Guidance documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAA41967-1C94-4DA4-B15A-95777A615ECA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$147</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="472">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1043,9 +1047,6 @@
   </si>
   <si>
     <t>wipe</t>
-  </si>
-  <si>
-    <t>spray (bag-on-valve)</t>
   </si>
   <si>
     <t>kit</t>
@@ -1411,11 +1412,184 @@
   <si>
     <t xml:space="preserve">solution pour irrigation </t>
   </si>
+  <si>
+    <t>pastille</t>
+  </si>
+  <si>
+    <t>liquide</t>
+  </si>
+  <si>
+    <t>éponge médicamenteuse</t>
+  </si>
+  <si>
+    <t>gaz médicinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+suspension buvable en gouttes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">émulsion buvable </t>
+  </si>
+  <si>
+    <t>pâte orale</t>
+  </si>
+  <si>
+    <t>poudre orale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solution buvable </t>
+  </si>
+  <si>
+    <t>suspension buvable</t>
+  </si>
+  <si>
+    <t>gélule orale à libération modifiée</t>
+  </si>
+  <si>
+    <t>comprimé oral à libération modifiée</t>
+  </si>
+  <si>
+    <t>solution pour bain de bouche</t>
+  </si>
+  <si>
+    <t>crème nasale</t>
+  </si>
+  <si>
+    <t>gel nasal</t>
+  </si>
+  <si>
+    <t>pommade nasale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poudre nasale </t>
+  </si>
+  <si>
+    <t>écouvillon</t>
+  </si>
+  <si>
+    <t>poudre pour suspension buvable</t>
+  </si>
+  <si>
+    <t>poudre pour solution buvable</t>
+  </si>
+  <si>
+    <t>poudre pour gouttes ophtalmique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bâton pour usage nasal </t>
+  </si>
+  <si>
+    <t>solution pour inhalation par nébuliseur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suspension pour inhalation par nébuliseur </t>
+  </si>
+  <si>
+    <t>crème ophtalmique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gel ophtalmique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+insert ophtalmique</t>
+  </si>
+  <si>
+    <t>pommade ophtalmique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+bandelette ophtalmique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+pommade auriculaire/ ophtalmique</t>
+  </si>
+  <si>
+    <t>comprimé orale</t>
+  </si>
+  <si>
+    <t>gouttes orales</t>
+  </si>
+  <si>
+    <t>gouttes ophtalmiques</t>
+  </si>
+  <si>
+    <t>spray nasal</t>
+  </si>
+  <si>
+    <t>capsule oral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">film orodispersible </t>
+  </si>
+  <si>
+    <t>comprimé orodispersible</t>
+  </si>
+  <si>
+    <t>gel buccal</t>
+  </si>
+  <si>
+    <t>pâte buccale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solution buccale </t>
+  </si>
+  <si>
+    <t>gel auriculaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+pommade auriculaire</t>
+  </si>
+  <si>
+    <t>bâton pour usage auriculaire</t>
+  </si>
+  <si>
+    <t>gel périodontal</t>
+  </si>
+  <si>
+    <t>ovule</t>
+  </si>
+  <si>
+    <t>emplâtre médicamenteux</t>
+  </si>
+  <si>
+    <t>poudre pour solution à diluer pour solution pour hémodialyse</t>
+  </si>
+  <si>
+    <t>poudre pour solution cutanée</t>
+  </si>
+  <si>
+    <t>poudre pour suspension intravésicale</t>
+  </si>
+  <si>
+    <t>poudre pour solution pour inhalation par nébuliseur</t>
+  </si>
+  <si>
+    <t>lingette</t>
+  </si>
+  <si>
+    <t>tampon imprégné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crème auriculaire </t>
+  </si>
+  <si>
+    <t>gouttes auriculaires</t>
+  </si>
+  <si>
+    <t>gouttes nasales</t>
+  </si>
+  <si>
+    <t>gouttes auriculaires/ophtalmiques</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1544,7 +1718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1552,7 +1726,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1879,2109 +2052,2258 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.26171875" customWidth="1"/>
+    <col min="4" max="4" width="27.83984375" customWidth="1"/>
+    <col min="5" max="5" width="54.578125" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="E1" s="27" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="16">
         <v>40007</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="16">
+        <v>40146</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>40146</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="16">
         <v>40079</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="E4" s="28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="16">
         <v>40108</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="E5" s="28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="16">
         <v>40111</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="29" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="E6" s="28" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="16">
         <v>40107</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="16">
+        <v>40112</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>40112</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="E8" s="28" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="16">
         <v>40113</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="E9" s="29" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="16">
         <v>40116</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="30" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="E10" s="29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="16">
         <v>40118</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="30" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="E11" s="29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="16">
         <v>40119</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="30" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+      <c r="E12" s="29" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="16">
         <v>40121</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="30" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="E13" s="29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="16">
         <v>40124</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="30" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="E14" s="29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="16">
         <v>40106</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="E15" s="29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="16">
         <v>40126</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="30" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="D16" s="11"/>
+      <c r="E16" s="29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="16">
         <v>40127</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="16">
+        <v>40010</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="29" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>40010</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="30" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="16">
         <v>40011</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="30" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="E19" s="29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="16">
         <v>40084</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="E20" s="29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="22">
         <v>40109</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>346</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="31" t="s">
+      <c r="C21" s="24" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="D21" s="26"/>
+      <c r="E21" s="30" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="16">
         <v>40082</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="30" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="E22" s="29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="16">
         <v>40142</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="30" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17">
+      <c r="E23" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="16">
         <v>40015</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="30" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
+      <c r="E24" s="29" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="16">
         <v>40033</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="30" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="E25" s="29" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="20">
         <v>40037</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="30" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="21">
+      <c r="E26" s="29" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="20">
         <v>40004</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="30" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="E27" s="29" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="20">
         <v>40048</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="20">
+        <v>40071</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="29" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
-        <v>40071</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="30" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
+    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="20">
         <v>40081</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+      <c r="E30" s="29" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="16">
         <v>40069</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="29" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="E31" s="28" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="16">
         <v>40068</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="30" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="E32" s="29" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="16">
         <v>40101</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>70</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="16">
         <v>40025</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="29" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+      <c r="E34" s="28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="16">
         <v>40022</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="29" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="D35" s="14"/>
+      <c r="E35" s="28" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="16">
         <v>40027</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="29" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+      <c r="E36" s="28" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="16">
         <v>40024</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>78</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="29" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="E37" s="28" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="16">
         <v>40034</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="E38" s="29" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="16">
         <v>40038</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>82</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="29" t="s">
+      <c r="E39" s="28" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="16">
+        <v>40041</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="29" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
-        <v>40041</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="30" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="16">
         <v>40042</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="29" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="E41" s="28" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="16">
         <v>40035</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="29" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="E42" s="28" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="22">
         <v>40006</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="E43" s="29"/>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="B43" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="E43" s="28"/>
+    </row>
+    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="16">
         <v>40115</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="23">
+      <c r="D44" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="22">
         <v>40114</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="25" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+      <c r="D45" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="16">
         <v>40073</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>95</v>
       </c>
       <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+      <c r="E46" s="28" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="16">
         <v>40130</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+      <c r="E47" s="28" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="16">
         <v>40023</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="29"/>
-    </row>
-    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+      <c r="E48" s="28" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="16">
         <v>40061</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+      <c r="E49" s="28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="16">
         <v>40080</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+      <c r="E50" s="28" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="16">
         <v>40003</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="11" t="s">
         <v>105</v>
       </c>
       <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="E51" s="28" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="16">
         <v>40046</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="11" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+      <c r="E52" s="28" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="16">
         <v>40043</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+      <c r="E53" s="28" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="16">
         <v>40044</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="11" t="s">
         <v>112</v>
       </c>
       <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="E54" s="28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="16">
         <v>40045</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+      <c r="E55" s="28" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="16">
         <v>40030</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="11" t="s">
         <v>116</v>
       </c>
       <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="E56" s="28" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="16">
         <v>40029</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+      <c r="E57" s="28" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="16">
         <v>40047</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="11" t="s">
         <v>121</v>
       </c>
       <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="E58" s="28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="16">
         <v>40031</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="11" t="s">
         <v>123</v>
       </c>
       <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="E59" s="28" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="16">
         <v>40028</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="11" t="s">
         <v>125</v>
       </c>
       <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="E60" s="28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="16">
         <v>40057</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="11" t="s">
         <v>127</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+      <c r="E61" s="28" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="16">
         <v>40050</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="11" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+      <c r="E62" s="28" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="16">
         <v>40051</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+      <c r="E63" s="28" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="16">
         <v>40052</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="11" t="s">
         <v>136</v>
       </c>
       <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="E64" s="29" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="16">
         <v>40053</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="11" t="s">
         <v>138</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+      <c r="E65" s="28" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="16">
         <v>40056</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="11" t="s">
         <v>141</v>
       </c>
       <c r="D66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+      <c r="E66" s="29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="16">
         <v>40058</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="E67" s="29"/>
-    </row>
-    <row r="68" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="E67" s="28" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="16">
         <v>40059</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="C68" s="12" t="s">
+      <c r="C68" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D68" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E68" s="29"/>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="E68" s="29" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="16">
         <v>40060</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+      <c r="E69" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="16">
         <v>40063</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D70" s="12" t="s">
+      <c r="C70" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="D70" s="11" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="E70" s="28" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="16">
         <v>40144</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D71" s="11"/>
+      <c r="E71" s="28" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="16">
+        <v>40145</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="D71" s="12"/>
-      <c r="E71" s="29" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
-        <v>40145</v>
-      </c>
-      <c r="B72" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="29"/>
-    </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+      <c r="D72" s="11"/>
+      <c r="E72" s="29" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="16">
         <v>40065</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="11" t="s">
         <v>148</v>
       </c>
       <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+      <c r="E73" s="28" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="16">
         <v>40067</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="11" t="s">
         <v>150</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="29" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="E74" s="28" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="16">
         <v>40072</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="11" t="s">
         <v>152</v>
       </c>
       <c r="D75" s="1"/>
-      <c r="E75" s="29" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
+      <c r="E75" s="28" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="16">
         <v>40075</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="11" t="s">
         <v>154</v>
       </c>
       <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
+      <c r="E76" s="29" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="16">
         <v>40074</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="11" t="s">
         <v>156</v>
       </c>
       <c r="D77" s="1"/>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
+      <c r="E77" s="28" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="16">
         <v>40064</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="11" t="s">
         <v>158</v>
       </c>
       <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
+      <c r="E78" s="28" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="16">
         <v>40070</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="11" t="s">
         <v>160</v>
       </c>
       <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
+      <c r="E79" s="28" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="16">
         <v>40078</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C80" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="11" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
+      <c r="E80" s="28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="16">
         <v>40066</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="11" t="s">
         <v>165</v>
       </c>
       <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
+      <c r="E81" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="16">
         <v>40076</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="11" t="s">
         <v>167</v>
       </c>
       <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="17">
+      <c r="E82" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="16">
         <v>40002</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="5" t="s">
         <v>169</v>
       </c>
       <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="17">
+      <c r="E83" s="28" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="16">
         <v>40009</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="C84" s="11" t="s">
         <v>171</v>
       </c>
       <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="17">
+      <c r="E84" s="28" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="16">
         <v>40008</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="E85" s="29"/>
-    </row>
-    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="17">
+      <c r="E85" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="16">
         <v>40005</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
+    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="16">
         <v>40089</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C87" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="17">
+      <c r="E87" s="28" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="16">
         <v>40086</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C88" s="12" t="s">
+      <c r="C88" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="11" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="17">
+      <c r="E88" s="28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="16">
         <v>40087</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C89" s="11" t="s">
         <v>182</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="17">
+      <c r="E89" s="28" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="16">
         <v>40088</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C90" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="17">
+      <c r="E90" s="29" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="16">
         <v>40090</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="C91" s="11" t="s">
         <v>188</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="17">
+      <c r="E91" s="28" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="16">
         <v>40117</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C92" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D92" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="D92" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="E92" s="29"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="17">
+      <c r="E92" s="28" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="16">
         <v>40102</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B93" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="11" t="s">
         <v>191</v>
       </c>
       <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="17">
+      <c r="E93" s="28" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="16">
         <v>40139</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C94" s="12" t="s">
+      <c r="C94" s="11" t="s">
         <v>193</v>
       </c>
       <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A95" s="17">
+      <c r="E94" s="28" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="16">
         <v>40120</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B95" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="C95" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D95" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="D95" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="E95" s="29"/>
-    </row>
-    <row r="96" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A96" s="17">
+      <c r="E95" s="28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="16">
         <v>40014</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C96" s="11" t="s">
         <v>195</v>
       </c>
       <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="17">
+      <c r="E96" s="29" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="16">
         <v>40122</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C97" s="12" t="s">
+      <c r="C97" s="11" t="s">
         <v>197</v>
       </c>
       <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="17">
+      <c r="E97" s="28" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="16">
         <v>40040</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C98" s="12" t="s">
+      <c r="C98" s="11" t="s">
         <v>199</v>
       </c>
       <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="17">
+      <c r="E98" s="28" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="16">
         <v>40026</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C99" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="17">
+      <c r="E99" s="28" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="16">
         <v>40054</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C100" s="12" t="s">
+      <c r="C100" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="11" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="17">
+      <c r="E100" s="28" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="16">
         <v>40049</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C101" s="12" t="s">
+      <c r="C101" s="11" t="s">
         <v>293</v>
       </c>
       <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
+      <c r="E101" s="29" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="21"/>
       <c r="B102" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C102" s="12" t="s">
+      <c r="C102" s="11" t="s">
         <v>292</v>
       </c>
       <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="17">
+      <c r="E102" s="29" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="16">
         <v>40085</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="C103" s="11" t="s">
         <v>208</v>
       </c>
       <c r="D103" s="1"/>
-      <c r="E103" s="29" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="17">
+      <c r="E103" s="28" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="16">
         <v>40018</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="C104" s="11" t="s">
         <v>210</v>
       </c>
       <c r="D104" s="1"/>
-      <c r="E104" s="29" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="17">
+      <c r="E104" s="28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="16">
         <v>40096</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C105" s="11" t="s">
         <v>212</v>
       </c>
       <c r="D105" s="1"/>
-      <c r="E105" s="29" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="17">
+      <c r="E105" s="28" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="16">
         <v>40017</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C106" s="12" t="s">
+      <c r="C106" s="11" t="s">
         <v>214</v>
       </c>
       <c r="D106" s="1"/>
-      <c r="E106" s="29" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="17">
+      <c r="E106" s="28" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="16">
         <v>40039</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="C107" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E107" s="29" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="17">
+      <c r="E107" s="28" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="16">
         <v>40016</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C108" s="12" t="s">
+      <c r="C108" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D108" s="1"/>
-      <c r="E108" s="29" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="17">
+      <c r="E108" s="28" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="16">
         <v>40021</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C109" s="11" t="s">
         <v>221</v>
       </c>
       <c r="D109" s="1"/>
-      <c r="E109" s="29" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="17">
+      <c r="E109" s="28" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="16">
         <v>40055</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C110" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C110" s="11" t="s">
         <v>222</v>
       </c>
       <c r="D110" s="1"/>
-      <c r="E110" s="29" t="s">
+      <c r="E110" s="28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="16">
+        <v>40062</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="16">
+        <v>40083</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="28" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="17">
-        <v>40062</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="29" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="17">
-        <v>40083</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C112" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="D112" s="1"/>
-      <c r="E112" s="29" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="17">
+    <row r="113" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="16">
         <v>40103</v>
       </c>
-      <c r="B113" s="16" t="s">
+      <c r="B113" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C113" s="12" t="s">
+      <c r="C113" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D113" s="6" t="s">
+      <c r="D113" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E113" s="30" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A114" s="17">
+      <c r="E113" s="29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="16">
         <v>40020</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C114" s="11" t="s">
         <v>229</v>
       </c>
       <c r="D114" s="1"/>
-      <c r="E114" s="30" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="17">
+      <c r="E114" s="29" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="16">
         <v>40099</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C115" s="12" t="s">
+      <c r="C115" s="11" t="s">
         <v>231</v>
       </c>
       <c r="D115" s="1"/>
-      <c r="E115" s="29" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="17">
+      <c r="E115" s="28" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="16">
         <v>40091</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C116" s="12" t="s">
+      <c r="C116" s="11" t="s">
         <v>233</v>
       </c>
       <c r="D116" s="1"/>
-      <c r="E116" s="30" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="17">
+      <c r="E116" s="29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="16">
         <v>40093</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="B117" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C117" s="12" t="s">
+      <c r="C117" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D117" s="12"/>
-      <c r="E117" s="30" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="17">
+      <c r="D117" s="11"/>
+      <c r="E117" s="29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="16">
         <v>40092</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C118" s="12" t="s">
+      <c r="C118" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="E118" s="29" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="17">
+      <c r="D118" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="E118" s="28" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="16">
         <v>40095</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C119" s="12" t="s">
+      <c r="C119" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E119" s="29" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="17">
+      <c r="E119" s="28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="16">
         <v>40094</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C120" s="12" t="s">
+      <c r="C120" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E120" s="30" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="17">
+      <c r="E120" s="29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="16">
         <v>40098</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C121" s="12" t="s">
+      <c r="C121" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E121" s="30" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="23">
+      <c r="E121" s="29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="22">
         <v>40140</v>
       </c>
-      <c r="B122" s="24" t="s">
+      <c r="B122" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C122" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="E122" s="29"/>
-    </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="17">
+      <c r="C122" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="E122" s="28"/>
+    </row>
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="16">
         <v>40123</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C123" s="12" t="s">
+      <c r="C123" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="E123" s="29" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="17">
+      <c r="E123" s="28" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="16">
         <v>40032</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C124" s="12" t="s">
+      <c r="C124" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E124" s="29" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="17">
+      <c r="E124" s="28" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="16">
         <v>40013</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C125" s="12" t="s">
+      <c r="C125" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="E125" s="29" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="17">
+      <c r="E125" s="28" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="16">
         <v>40001</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C126" s="12" t="s">
+      <c r="C126" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E126" s="29" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A127" s="17">
+      <c r="E126" s="28" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="16">
         <v>40036</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C127" s="12" t="s">
+      <c r="C127" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E127" s="29" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="17">
-        <v>40125</v>
-      </c>
-      <c r="B128" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="C128" s="12"/>
-      <c r="E128" s="29"/>
-    </row>
-    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="17">
+      <c r="E127" s="28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="16">
         <v>40104</v>
       </c>
+      <c r="B128" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E128" s="28" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="16">
+        <v>40105</v>
+      </c>
       <c r="B129" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C129" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="E129" s="29" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="17">
-        <v>40105</v>
+        <v>256</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E129" s="28" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="16">
+        <v>40097</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C130" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="E130" s="29" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="17">
-        <v>40097</v>
+        <v>258</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="16">
+        <v>40019</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C131" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="E131" s="29" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="17">
-        <v>40019</v>
-      </c>
-      <c r="B132" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C132" s="12" t="s">
+      <c r="C131" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E132" s="29" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="17">
+      <c r="E131" s="28" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="16">
         <v>40128</v>
       </c>
-      <c r="B133" s="20" t="s">
+      <c r="B132" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="C133" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="D133" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="E133" s="29"/>
-    </row>
-    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" s="23">
+      <c r="C132" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="D132" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="E132" s="28" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="22">
         <v>40077</v>
       </c>
-      <c r="B134" s="26" t="s">
+      <c r="B133" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C134" s="25" t="s">
+      <c r="C133" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="D134" s="23" t="s">
-        <v>373</v>
-      </c>
-      <c r="E134" s="32" t="s">
+      <c r="D133" s="22" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="17">
+      <c r="E133" s="31" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="16">
         <v>40100</v>
       </c>
-      <c r="B135" s="18" t="s">
+      <c r="B134" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="C134" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="E135" s="29" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="17">
+      <c r="E134" s="28" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="16">
         <v>40012</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C136" s="12" t="s">
+      <c r="C135" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E136" s="29" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A137" s="17">
+      <c r="E135" s="28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="16">
         <v>40132</v>
       </c>
-      <c r="B137" s="7" t="s">
+      <c r="B136" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C137" s="12" t="s">
+      <c r="C136" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E137" s="29" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A138" s="17">
+      <c r="E136" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="16">
         <v>40133</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C138" s="12" t="s">
+      <c r="C137" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E138" s="29" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="17">
+      <c r="E137" s="28" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="16">
         <v>40135</v>
       </c>
-      <c r="B139" s="7" t="s">
+      <c r="B138" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C139" s="12" t="s">
+      <c r="C138" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E139" s="29" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A140" s="17">
+      <c r="E138" s="28" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="16">
         <v>40134</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B139" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C140" s="12" t="s">
+      <c r="C139" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E140" s="29" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="17">
+      <c r="E139" s="28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="16">
         <v>40131</v>
       </c>
+      <c r="B140" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C140" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E140" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="16">
+        <v>40137</v>
+      </c>
       <c r="B141" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A142" s="17">
-        <v>40137</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E142" s="30" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" s="17">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="16">
         <v>40136</v>
       </c>
-      <c r="B143" s="9" t="s">
+      <c r="B142" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C143" s="12" t="s">
+      <c r="C142" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="E143" s="29" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="17">
+      <c r="E142" s="28" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="16">
         <v>40138</v>
       </c>
+      <c r="B143" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C143" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E143" s="28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="16">
+        <v>40141</v>
+      </c>
       <c r="B144" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C144" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="E144" s="29" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="17">
-        <v>40141</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C145" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="E145" s="30" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="17">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="16">
         <v>40129</v>
       </c>
-      <c r="B146" s="20" t="s">
+      <c r="B145" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C146" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="D146" s="17" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="5"/>
-      <c r="C147" s="1"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="26" t="s">
+      <c r="C145" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="E145" s="28" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B146" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="C146" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C148" s="12" t="s">
+      <c r="E146" s="28" t="s">
         <v>378</v>
-      </c>
-      <c r="E148" s="29" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CCDD Dosage Form Concepts
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAA41967-1C94-4DA4-B15A-95777A615ECA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B71D6F2A-CF66-46B5-9ED1-D7A1814C2EAD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$149</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="478">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1584,6 +1584,25 @@
   </si>
   <si>
     <t>gouttes auriculaires/ophtalmiques</t>
+  </si>
+  <si>
+    <t>Liquid sterile preparation consisting of a solution intended for administration by injection; the active substance(s) are released over an extended period of time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+solution injectable à libération prolongée</t>
+  </si>
+  <si>
+    <t>Solid sterile preparation consisting of one or more powders, including freeze-dried powders, intended to be dispersed in the specified liquid to obtain a prolonged-release solution for injection</t>
+  </si>
+  <si>
+    <t>Not currently present in EDQM but uses EDQM pattern</t>
+  </si>
+  <si>
+    <t>poudre pour solution injectable à libération prolongée</t>
+  </si>
+  <si>
+    <t>prolonged-release solution for injection</t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3679,630 +3698,656 @@
         <v>406</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="16">
-        <v>40018</v>
-      </c>
-      <c r="B104" s="4" t="s">
+    <row r="104" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B104" s="17" t="s">
         <v>209</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D104" s="1"/>
+        <v>474</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="E104" s="28" t="s">
-        <v>404</v>
+        <v>476</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="16">
-        <v>40096</v>
+        <v>40018</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="28" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="16">
-        <v>40017</v>
+        <v>40096</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="28" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="16">
+        <v>40017</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="28" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="16">
+    <row r="108" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="16">
         <v>40039</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C108" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D107" s="11" t="s">
+      <c r="D108" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E107" s="28" t="s">
+      <c r="E108" s="28" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="16">
-        <v>40016</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="28" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="16">
-        <v>40021</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="28" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="16">
-        <v>40055</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>308</v>
+        <v>40021</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="16">
-        <v>40062</v>
+        <v>40055</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="28" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="16">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="16">
+        <v>40083</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D113" s="1"/>
+      <c r="E113" s="28" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="16">
-        <v>40103</v>
-      </c>
-      <c r="B113" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E113" s="29" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="16">
+        <v>40103</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E114" s="29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B115" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D115" s="5"/>
+      <c r="E115" s="29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="16">
         <v>40020</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C116" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="D114" s="1"/>
-      <c r="E114" s="29" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="16">
-        <v>40099</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="28" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="16">
-        <v>40091</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="29" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="16">
-        <v>40093</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>234</v>
+        <v>40099</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="D117" s="11"/>
-      <c r="E117" s="29" t="s">
-        <v>389</v>
+        <v>231</v>
+      </c>
+      <c r="D117" s="1"/>
+      <c r="E117" s="28" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="16">
-        <v>40092</v>
+        <v>40091</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="E118" s="28" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>233</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="16">
-        <v>40095</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>238</v>
+        <v>40093</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="E119" s="28" t="s">
-        <v>388</v>
+        <v>235</v>
+      </c>
+      <c r="D119" s="11"/>
+      <c r="E119" s="29" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="16">
-        <v>40094</v>
+        <v>40092</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="E120" s="29" t="s">
-        <v>387</v>
+        <v>237</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="E120" s="28" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="16">
-        <v>40098</v>
+        <v>40095</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="E121" s="29" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="22">
-        <v>40140</v>
-      </c>
-      <c r="B122" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="C122" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="E122" s="28"/>
+        <v>239</v>
+      </c>
+      <c r="E121" s="28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="16">
+        <v>40094</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E122" s="29" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="16">
-        <v>40123</v>
+        <v>40098</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E123" s="28" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="16">
-        <v>40032</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="E124" s="28" t="s">
-        <v>384</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="E123" s="29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="22">
+        <v>40140</v>
+      </c>
+      <c r="B124" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="C124" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="E124" s="28"/>
     </row>
     <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="16">
-        <v>40013</v>
+        <v>40123</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E125" s="28" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="16">
-        <v>40001</v>
+        <v>40032</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E126" s="28" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="16">
-        <v>40036</v>
+        <v>40013</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E127" s="28" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="16">
-        <v>40104</v>
+        <v>40001</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E128" s="28" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="16">
-        <v>40105</v>
+        <v>40036</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E129" s="28" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="16">
+        <v>40104</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="16">
+        <v>40105</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E131" s="28" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="16">
         <v>40097</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C132" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E130" s="28" t="s">
+      <c r="E132" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="16">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="16">
         <v>40019</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C131" s="11" t="s">
+      <c r="C133" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E131" s="28" t="s">
+      <c r="E133" s="28" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="16">
+    <row r="134" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="16">
         <v>40128</v>
       </c>
-      <c r="B132" s="19" t="s">
+      <c r="B134" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C134" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="D132" s="16" t="s">
+      <c r="D134" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="E132" s="28" t="s">
+      <c r="E134" s="28" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="22">
+    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="22">
         <v>40077</v>
       </c>
-      <c r="B133" s="25" t="s">
+      <c r="B135" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C133" s="24" t="s">
+      <c r="C135" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="D133" s="22" t="s">
+      <c r="D135" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="E133" s="31" t="s">
+      <c r="E135" s="31" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="16">
+    <row r="136" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="16">
         <v>40100</v>
       </c>
-      <c r="B134" s="17" t="s">
+      <c r="B136" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C136" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="E134" s="28" t="s">
+      <c r="E136" s="28" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="16">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="16">
         <v>40012</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C137" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E135" s="28" t="s">
+      <c r="E137" s="28" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="16">
+    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="16">
         <v>40132</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B138" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C138" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E136" s="28" t="s">
+      <c r="E138" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="16">
+    <row r="139" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="16">
         <v>40133</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C139" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E137" s="28" t="s">
+      <c r="E139" s="28" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="16">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="16">
         <v>40135</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B140" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C140" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E138" s="28" t="s">
+      <c r="E140" s="28" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="16">
+    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="16">
         <v>40134</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B141" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C141" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E139" s="28" t="s">
+      <c r="E141" s="28" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="16">
-        <v>40131</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C140" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="E140" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="16">
-        <v>40137</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C141" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="E141" s="29" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="16">
-        <v>40136</v>
-      </c>
-      <c r="B142" s="8" t="s">
-        <v>278</v>
+        <v>40131</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E142" s="28" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="16">
-        <v>40138</v>
+        <v>40137</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="E143" s="28" t="s">
-        <v>360</v>
+        <v>277</v>
+      </c>
+      <c r="E143" s="29" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="16">
+        <v>40136</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E144" s="28" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="16">
+        <v>40138</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E145" s="28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="16">
         <v>40141</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C146" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="E144" s="29" t="s">
+      <c r="E146" s="29" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="16">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="16">
         <v>40129</v>
       </c>
-      <c r="B145" s="19" t="s">
+      <c r="B147" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C147" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="D145" s="16" t="s">
+      <c r="D147" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="E145" s="28" t="s">
+      <c r="E147" s="28" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B146" s="25" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B148" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C148" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="E146" s="28" t="s">
+      <c r="E148" s="28" t="s">
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CCDD Dosage Form Concepts: Line 104 prolonged-release solution
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B71D6F2A-CF66-46B5-9ED1-D7A1814C2EAD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CFD614-E53A-4070-803A-E14D243E4B58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="479">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1603,6 +1603,9 @@
   </si>
   <si>
     <t>prolonged-release solution for injection</t>
+  </si>
+  <si>
+    <t>powder for prolonged-release solution for injection</t>
   </si>
 </sst>
 </file>
@@ -2074,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3700,7 +3703,7 @@
     </row>
     <row r="104" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" s="17" t="s">
-        <v>209</v>
+        <v>478</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>474</v>

</xml_diff>

<commit_message>
CCDD Dosage form concepts - new version uploaded
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CFD614-E53A-4070-803A-E14D243E4B58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC8CC685-1D34-4D56-A5EB-4993202EF7DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$150</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="482">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1034,12 +1034,6 @@
     <t>pad</t>
   </si>
   <si>
-    <t>oral drops, solution</t>
-  </si>
-  <si>
-    <t>oral drops, suspension</t>
-  </si>
-  <si>
     <t>ring (slow release)</t>
   </si>
   <si>
@@ -1159,9 +1153,6 @@
   <si>
     <t xml:space="preserve">  
 bâton pour application cutanée</t>
-  </si>
-  <si>
-    <t>suspension pour application cutanée</t>
   </si>
   <si>
     <t>gel dentaire</t>
@@ -1606,6 +1597,24 @@
   </si>
   <si>
     <t>powder for prolonged-release solution for injection</t>
+  </si>
+  <si>
+    <t>oral drops solution</t>
+  </si>
+  <si>
+    <t>oral drops suspension</t>
+  </si>
+  <si>
+    <t>cutaneous spray powder</t>
+  </si>
+  <si>
+    <t>Solid, usually multidose preparation presented in a pressurised container with a spray valve or in a container equipped with a spray pump.  The spray is intended for cutaneous use</t>
+  </si>
+  <si>
+    <t>EDQM</t>
+  </si>
+  <si>
+    <t>poudre pour pulvérisation cutanée</t>
   </si>
 </sst>
 </file>
@@ -2075,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2104,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2119,7 +2128,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2130,10 +2139,10 @@
         <v>295</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2150,7 +2159,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2167,7 +2176,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2182,7 +2191,7 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="28" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2197,7 +2206,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="29" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2211,10 +2220,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2231,7 +2240,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2248,7 +2257,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2263,7 +2272,7 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2278,7 +2287,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2293,7 +2302,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2308,7 +2317,7 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="29" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2325,2033 +2334,2045 @@
         <v>33</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="16">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="16">
         <v>40126</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="29" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="16">
-        <v>40127</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="16">
-        <v>40010</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>40127</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="29" t="s">
-        <v>342</v>
-      </c>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="16">
-        <v>40011</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>40010</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="29" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="16">
+        <v>40011</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="16">
         <v>40084</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="29" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="22">
+      <c r="E21" s="29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="22">
         <v>40109</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B22" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>345</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="30" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="16">
-        <v>40082</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>351</v>
+      <c r="C22" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="30" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="16">
+        <v>40082</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="16">
         <v>40142</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="29" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="16">
-        <v>40015</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="29" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="16">
-        <v>40033</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>51</v>
+        <v>40015</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A26" s="16">
+        <v>40033</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="20">
+        <v>40037</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="20">
+        <v>40004</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="29" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="20">
+        <v>40048</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="29" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="20">
-        <v>40037</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="29" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="20">
+        <v>40071</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="29" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="20">
-        <v>40004</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="29" t="s">
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="20">
+        <v>40081</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="29" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="20">
-        <v>40048</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="20">
-        <v>40071</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="29" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="20">
-        <v>40081</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="16">
-        <v>40069</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="28" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="16">
+        <v>40069</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="16">
         <v>40068</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="29" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="16">
-        <v>40101</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="28" t="s">
-        <v>69</v>
+      <c r="E33" s="29" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="16">
-        <v>40025</v>
+        <v>40101</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="28" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="16">
-        <v>40022</v>
+        <v>40025</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="14"/>
+        <v>71</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="28" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="16">
-        <v>40027</v>
+        <v>40022</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="14"/>
       <c r="E36" s="28" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16">
-        <v>40024</v>
+        <v>40027</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="28" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="16">
-        <v>40034</v>
+        <v>40024</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="29" t="s">
-        <v>411</v>
+      <c r="E38" s="28" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="16">
-        <v>40038</v>
+        <v>40034</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="28" t="s">
-        <v>412</v>
+      <c r="E39" s="29" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="16">
+        <v>40038</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="28" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="16">
         <v>40041</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="29" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="16">
-        <v>40042</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>414</v>
+      <c r="D41" s="1"/>
+      <c r="E41" s="29" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="16">
+        <v>40042</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="16">
         <v>40035</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="28" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="22">
+      <c r="D43" s="1"/>
+      <c r="E43" s="28" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="22">
         <v>40006</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>375</v>
-      </c>
-      <c r="E43" s="28"/>
-    </row>
-    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="16">
+      <c r="B44" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="E44" s="28"/>
+    </row>
+    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="16">
         <v>40115</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="22">
+      <c r="D45" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="22">
         <v>40114</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B46" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C46" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="E45" s="28" t="s">
+      <c r="D46" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="E46" s="28" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="16">
-        <v>40073</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="28" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="16">
-        <v>40130</v>
+        <v>40073</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="28" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="16">
+        <v>40130</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="28" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="16">
         <v>40023</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B49" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="28" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="16">
+      <c r="E49" s="28" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="16">
         <v>40061</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="16">
-        <v>40080</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>102</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="16">
-        <v>40003</v>
+        <v>40080</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="E51" s="28" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="16">
-        <v>40046</v>
+        <v>40003</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="28" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="16">
+        <v>40046</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="16">
         <v>40043</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C54" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E53" s="28" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="16">
-        <v>40044</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="1"/>
       <c r="E54" s="28" t="s">
-        <v>430</v>
+        <v>467</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="16">
-        <v>40045</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>113</v>
+        <v>40044</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="28" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="16">
-        <v>40030</v>
+        <v>40045</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="28" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="16">
+        <v>40030</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="28" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="16">
         <v>40029</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C58" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E57" s="28" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="16">
+      <c r="E58" s="28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="16">
         <v>40047</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C59" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="28" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="16">
-        <v>40031</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="28" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="16">
-        <v>40028</v>
+        <v>40031</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="28" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="16">
+        <v>40028</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="28" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="16">
         <v>40057</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="28" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="16">
+      <c r="E62" s="28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="16">
         <v>40050</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C63" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D63" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="28" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="16">
-        <v>40051</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E63" s="28" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="16">
-        <v>40052</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>135</v>
+        <v>40051</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="29" t="s">
-        <v>442</v>
+        <v>133</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="16">
-        <v>40053</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>137</v>
+        <v>40052</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E65" s="28" t="s">
-        <v>443</v>
+        <v>136</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="29" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="16">
+        <v>40053</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" s="28" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="16">
         <v>40056</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C67" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="29" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="16">
+      <c r="D67" s="1"/>
+      <c r="E67" s="29" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="16">
         <v>40058</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B68" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C68" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D68" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="E67" s="28" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="16">
+      <c r="E68" s="28" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="16">
         <v>40059</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B69" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C69" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D69" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="16">
-        <v>40060</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="28" t="s">
-        <v>450</v>
+      <c r="E69" s="29" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="16">
-        <v>40063</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>145</v>
+        <v>40060</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>322</v>
+        <v>143</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E70" s="28" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="16">
-        <v>40144</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>300</v>
+        <v>40063</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="D71" s="11"/>
+        <v>320</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="E71" s="28" t="s">
-        <v>349</v>
+        <v>444</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="16">
+        <v>40144</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D72" s="11"/>
+      <c r="E72" s="28" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="16">
         <v>40145</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="D72" s="11"/>
-      <c r="E72" s="29" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="16">
-        <v>40065</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>147</v>
+      <c r="B73" s="19" t="s">
+        <v>477</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="28" t="s">
-        <v>421</v>
+        <v>317</v>
+      </c>
+      <c r="D73" s="11"/>
+      <c r="E73" s="29" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="16">
-        <v>40067</v>
+        <v>40065</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="28" t="s">
-        <v>350</v>
+        <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="16">
-        <v>40072</v>
+        <v>40067</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="28" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="16">
+        <v>40072</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="16">
         <v>40075</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C77" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="29" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="16">
-        <v>40074</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="28" t="s">
-        <v>423</v>
+      <c r="E77" s="29" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="16">
-        <v>40064</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>157</v>
+        <v>40074</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="28" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="16">
-        <v>40070</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>159</v>
+        <v>40064</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="28" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="16">
+        <v>40070</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="28" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="16">
         <v>40078</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C81" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E80" s="28" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="16">
-        <v>40066</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D81" s="1"/>
       <c r="E81" s="28" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="16">
-        <v>40076</v>
+        <v>40066</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="28" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="16">
-        <v>40002</v>
+        <v>40076</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>167</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="28" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="16">
-        <v>40009</v>
+        <v>40002</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="16">
+        <v>40009</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="16">
+        <v>40008</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="16">
+        <v>40005</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="16">
+        <v>40089</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="16">
+        <v>40086</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="16">
+        <v>40087</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="16">
+        <v>40088</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E91" s="29" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="16">
-        <v>40008</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="E85" s="28" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="16">
+        <v>40090</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E92" s="28" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="16">
-        <v>40005</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="16">
-        <v>40089</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E87" s="28" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="16">
-        <v>40086</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E88" s="28" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="16">
-        <v>40087</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E89" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="16">
-        <v>40088</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E90" s="29" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="16">
-        <v>40090</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E91" s="28" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="16">
+    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="16">
         <v>40117</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="B93" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="C92" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="E92" s="28" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="16">
+      <c r="C93" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="16">
         <v>40102</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B94" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="D93" s="1"/>
-      <c r="E93" s="28" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="16">
-        <v>40139</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="28" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="16">
+        <v>40139</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="28" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="16">
         <v>40120</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B96" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C95" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="E95" s="28" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="16">
+      <c r="C96" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="E96" s="28" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="16">
         <v>40014</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C97" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="D96" s="1"/>
-      <c r="E96" s="29" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="16">
-        <v>40122</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>197</v>
-      </c>
       <c r="D97" s="1"/>
-      <c r="E97" s="28" t="s">
-        <v>463</v>
+      <c r="E97" s="29" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="16">
-        <v>40040</v>
+        <v>40122</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="28" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="16">
-        <v>40026</v>
+        <v>40040</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="28" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="16">
+        <v>40026</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="28" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="16">
         <v>40054</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C101" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E100" s="28" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="16">
+      <c r="E101" s="28" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="16">
         <v>40049</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C102" s="11" t="s">
         <v>293</v>
-      </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="29" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="21"/>
-      <c r="B102" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>292</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="29" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="16">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="21"/>
+      <c r="B103" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="29" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="16">
         <v>40085</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C104" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D103" s="1"/>
-      <c r="E103" s="28" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B104" s="17" t="s">
-        <v>478</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="D104" s="11" t="s">
+      <c r="D104" s="1"/>
+      <c r="E104" s="28" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105" s="17" t="s">
         <v>475</v>
       </c>
-      <c r="E104" s="28" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="16">
-        <v>40018</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>209</v>
-      </c>
       <c r="C105" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D105" s="1"/>
+        <v>471</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>472</v>
+      </c>
       <c r="E105" s="28" t="s">
-        <v>404</v>
+        <v>473</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="16">
-        <v>40096</v>
+        <v>40018</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="16">
-        <v>40017</v>
+        <v>40096</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="28" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="16">
+        <v>40017</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="16">
         <v>40039</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C109" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D109" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E108" s="28" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="16">
-        <v>40016</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D109" s="1"/>
       <c r="E109" s="28" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="16">
-        <v>40021</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="28" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="16">
-        <v>40055</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>308</v>
+        <v>40021</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="28" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="16">
-        <v>40062</v>
+        <v>40055</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>306</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="28" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="16">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="28" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="16">
+        <v>40083</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D114" s="1"/>
+      <c r="E114" s="28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="16">
         <v>40103</v>
       </c>
-      <c r="B114" s="15" t="s">
+      <c r="B115" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C115" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E114" s="29" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B115" s="17" t="s">
-        <v>477</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="D115" s="5"/>
       <c r="E115" s="29" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="16">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B116" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="D116" s="5"/>
+      <c r="E116" s="29" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="16">
         <v>40020</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C117" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D116" s="1"/>
-      <c r="E116" s="29" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="16">
-        <v>40099</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>231</v>
-      </c>
       <c r="D117" s="1"/>
-      <c r="E117" s="28" t="s">
-        <v>394</v>
+      <c r="E117" s="29" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="16">
+        <v>40099</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="28" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="16">
         <v>40091</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C119" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D118" s="1"/>
-      <c r="E118" s="29" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="16">
+      <c r="D119" s="1"/>
+      <c r="E119" s="29" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="16">
         <v>40093</v>
       </c>
-      <c r="B119" s="6" t="s">
+      <c r="B120" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C120" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D119" s="11"/>
-      <c r="E119" s="29" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="16">
-        <v>40092</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="E120" s="28" t="s">
-        <v>392</v>
+      <c r="D120" s="11"/>
+      <c r="E120" s="29" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="16">
-        <v>40095</v>
+        <v>40092</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>387</v>
       </c>
       <c r="E121" s="28" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="16">
-        <v>40094</v>
+        <v>40095</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="E122" s="29" t="s">
-        <v>387</v>
+        <v>239</v>
+      </c>
+      <c r="E122" s="28" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="16">
+        <v>40094</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E123" s="29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="16">
         <v>40098</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C124" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E123" s="29" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="22">
+      <c r="E124" s="29" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="22">
         <v>40140</v>
       </c>
-      <c r="B124" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="C124" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="E124" s="28"/>
-    </row>
-    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="16">
-        <v>40123</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C125" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E125" s="28" t="s">
-        <v>385</v>
-      </c>
+      <c r="B125" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="E125" s="28"/>
     </row>
     <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="16">
-        <v>40032</v>
+        <v>40123</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E126" s="28" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="16">
+        <v>40032</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E127" s="28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="16">
         <v>40013</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C128" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="E127" s="28" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="16">
+      <c r="E128" s="28" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="16">
         <v>40001</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C129" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E128" s="28" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="16">
-        <v>40036</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C129" s="11" t="s">
-        <v>253</v>
-      </c>
       <c r="E129" s="28" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="16">
-        <v>40104</v>
+        <v>40036</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E130" s="28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="16">
-        <v>40105</v>
+        <v>40104</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E131" s="28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="16">
+        <v>40105</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C132" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E132" s="28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="16">
         <v>40097</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C133" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E132" s="28" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="16">
+      <c r="E133" s="28" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="16">
         <v>40019</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C134" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E133" s="28" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="16">
+      <c r="E134" s="28" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="16">
         <v>40128</v>
       </c>
-      <c r="B134" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="D134" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="E134" s="28" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="22">
+      <c r="B135" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="E135" s="28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="22">
         <v>40077</v>
       </c>
-      <c r="B135" s="25" t="s">
+      <c r="B136" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C135" s="24" t="s">
+      <c r="C136" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="D135" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="E135" s="31" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="16">
+      <c r="D136" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="E136" s="31" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="16">
         <v>40100</v>
       </c>
-      <c r="B136" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="C136" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="E136" s="28" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="16">
+      <c r="B137" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="E137" s="28" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="16">
         <v>40012</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C138" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E137" s="28" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="16">
+      <c r="E138" s="28" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="16">
         <v>40132</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B139" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C139" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E138" s="28" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="16">
+      <c r="E139" s="28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="16">
         <v>40133</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C140" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E139" s="28" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="16">
+      <c r="E140" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="16">
         <v>40135</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B141" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C141" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E140" s="28" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="16">
-        <v>40134</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C141" s="11" t="s">
-        <v>273</v>
-      </c>
       <c r="E141" s="28" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="16">
+        <v>40134</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E142" s="28" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="16">
         <v>40131</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C143" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="E142" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="16">
+      <c r="E143" s="28" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="16">
         <v>40137</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C144" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="E143" s="29" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="16">
-        <v>40136</v>
-      </c>
-      <c r="B144" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="C144" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="E144" s="28" t="s">
-        <v>362</v>
+      <c r="E144" s="29" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="16">
-        <v>40138</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>280</v>
+        <v>40136</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E145" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="16">
+        <v>40138</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C146" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E146" s="28" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="16">
         <v>40141</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C147" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="E146" s="29" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="16">
+      <c r="E147" s="29" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="16">
         <v>40129</v>
       </c>
-      <c r="B147" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="D147" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="E147" s="28" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B148" s="25" t="s">
-        <v>376</v>
+      <c r="B148" s="19" t="s">
+        <v>302</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>377</v>
+        <v>318</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>313</v>
       </c>
       <c r="E148" s="28" t="s">
-        <v>378</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B149" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E149" s="28" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CCDD NTP Dosage form concepts.xlsx
Added powder for solution for intraocular irrigation
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC8CC685-1D34-4D56-A5EB-4993202EF7DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4404"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$151</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="485">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1616,11 +1610,20 @@
   <si>
     <t>poudre pour pulvérisation cutanée</t>
   </si>
+  <si>
+    <t>powder for solution for intraocular injection</t>
+  </si>
+  <si>
+    <t>Solid sterile preparation consisting of one or more powders, including freeze-dried powders, intended to be dissolved in the specified liquid to obtain a solution for intraocular irrigation.</t>
+  </si>
+  <si>
+    <t>Poudre pour solution pour irrigation intraoculaire</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2076,27 +2079,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.26171875" customWidth="1"/>
-    <col min="4" max="4" width="27.83984375" customWidth="1"/>
-    <col min="5" max="5" width="54.578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2116,7 +2119,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>40007</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>40079</v>
       </c>
@@ -2162,7 +2165,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>40108</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>40111</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>40107</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>40112</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>40113</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>40116</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>40118</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>40119</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>40121</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>40124</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>40106</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>478</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>40126</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>40084</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>40082</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>40142</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>40037</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>40048</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>40071</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>40081</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>40069</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>40068</v>
       </c>
@@ -2644,7 +2647,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>40022</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>40027</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>40038</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>40041</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>40042</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>40130</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>40023</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>40061</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>40080</v>
       </c>
@@ -2908,7 +2911,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>40046</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>40047</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>40031</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>40028</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>40057</v>
       </c>
@@ -3243,7 +3246,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="16">
         <v>40065</v>
       </c>
@@ -3288,7 +3291,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="16">
         <v>40075</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="16">
         <v>40078</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="16">
         <v>40076</v>
       </c>
@@ -3410,7 +3413,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="16">
         <v>40009</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="16">
         <v>40089</v>
       </c>
@@ -3521,7 +3524,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="16">
         <v>40090</v>
       </c>
@@ -3538,7 +3541,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="16">
         <v>40117</v>
       </c>
@@ -3555,7 +3558,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="16">
         <v>40102</v>
       </c>
@@ -3585,7 +3588,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="16">
         <v>40120</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="16">
         <v>40014</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="16">
         <v>40122</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="16">
         <v>40040</v>
       </c>
@@ -3647,7 +3650,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="16">
         <v>40026</v>
       </c>
@@ -3722,7 +3725,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B105" s="17" t="s">
         <v>475</v>
       </c>
@@ -3736,7 +3739,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="16">
         <v>40018</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="16">
         <v>40017</v>
       </c>
@@ -3781,597 +3784,609 @@
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="16">
+    <row r="109" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A109" s="21"/>
+      <c r="B109" s="17" t="s">
+        <v>482</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="E109" s="28" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="16">
         <v>40039</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C110" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D109" s="11" t="s">
+      <c r="D110" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E109" s="28" t="s">
+      <c r="E110" s="28" t="s">
         <v>400</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="16">
-        <v>40016</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="28" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="16">
-        <v>40021</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="16">
-        <v>40055</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>306</v>
+        <v>40021</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="28" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="16">
-        <v>40062</v>
+        <v>40055</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="28" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114" s="16">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="28" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A115" s="16">
+        <v>40083</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D115" s="1"/>
+      <c r="E115" s="28" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="16">
+    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="16">
         <v>40103</v>
       </c>
-      <c r="B115" s="15" t="s">
+      <c r="B116" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C116" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D116" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E115" s="29" t="s">
+      <c r="E116" s="29" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B116" s="17" t="s">
+    <row r="117" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B117" s="17" t="s">
         <v>474</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C117" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="D116" s="5"/>
-      <c r="E116" s="29" t="s">
+      <c r="D117" s="5"/>
+      <c r="E117" s="29" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="16">
+    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A118" s="16">
         <v>40020</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C118" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D117" s="1"/>
-      <c r="E117" s="29" t="s">
+      <c r="D118" s="1"/>
+      <c r="E118" s="29" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="16">
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A119" s="16">
         <v>40099</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C119" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="D118" s="1"/>
-      <c r="E118" s="28" t="s">
+      <c r="D119" s="1"/>
+      <c r="E119" s="28" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="16">
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="16">
         <v>40091</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C120" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D119" s="1"/>
-      <c r="E119" s="29" t="s">
+      <c r="D120" s="1"/>
+      <c r="E120" s="29" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="16">
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A121" s="16">
         <v>40093</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B121" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C121" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D120" s="11"/>
-      <c r="E120" s="29" t="s">
+      <c r="D121" s="11"/>
+      <c r="E121" s="29" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="16">
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A122" s="16">
         <v>40092</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C122" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="D121" s="11" t="s">
+      <c r="D122" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E121" s="28" t="s">
+      <c r="E122" s="28" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="16">
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A123" s="16">
         <v>40095</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C123" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E122" s="28" t="s">
+      <c r="E123" s="28" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="16">
+    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A124" s="16">
         <v>40094</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C124" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E123" s="29" t="s">
+      <c r="E124" s="29" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="16">
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="16">
         <v>40098</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C125" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E124" s="29" t="s">
+      <c r="E125" s="29" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="22">
+    <row r="126" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="22">
         <v>40140</v>
       </c>
-      <c r="B125" s="23" t="s">
+      <c r="B126" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="C125" s="24" t="s">
+      <c r="C126" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E125" s="28"/>
-    </row>
-    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="16">
+      <c r="E126" s="28"/>
+    </row>
+    <row r="127" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A127" s="16">
         <v>40123</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C127" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="E126" s="28" t="s">
+      <c r="E127" s="28" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="16">
+    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A128" s="16">
         <v>40032</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C128" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E127" s="28" t="s">
+      <c r="E128" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="16">
+    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A129" s="16">
         <v>40013</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C129" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="E128" s="28" t="s">
+      <c r="E129" s="28" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="16">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="16">
         <v>40001</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C129" s="11" t="s">
+      <c r="C130" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E129" s="28" t="s">
+      <c r="E130" s="28" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="16">
+    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A131" s="16">
         <v>40036</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C131" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E130" s="28" t="s">
+      <c r="E131" s="28" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="16">
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A132" s="16">
         <v>40104</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C131" s="11" t="s">
+      <c r="C132" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E131" s="28" t="s">
+      <c r="E132" s="28" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="16">
+    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A133" s="16">
         <v>40105</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C133" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E132" s="28" t="s">
+      <c r="E133" s="28" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="16">
+    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A134" s="16">
         <v>40097</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C134" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E133" s="28" t="s">
+      <c r="E134" s="28" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="16">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" s="16">
         <v>40019</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C135" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E134" s="28" t="s">
+      <c r="E135" s="28" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="16">
+    <row r="136" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="16">
         <v>40128</v>
       </c>
-      <c r="B135" s="19" t="s">
+      <c r="B136" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C136" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D135" s="16" t="s">
+      <c r="D136" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E135" s="28" t="s">
+      <c r="E136" s="28" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="22">
+    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A137" s="22">
         <v>40077</v>
       </c>
-      <c r="B136" s="25" t="s">
+      <c r="B137" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C136" s="24" t="s">
+      <c r="C137" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="D136" s="22" t="s">
+      <c r="D137" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="E136" s="31" t="s">
+      <c r="E137" s="31" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="16">
+    <row r="138" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A138" s="16">
         <v>40100</v>
       </c>
-      <c r="B137" s="17" t="s">
+      <c r="B138" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C138" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="E137" s="28" t="s">
+      <c r="E138" s="28" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="16">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" s="16">
         <v>40012</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C139" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E138" s="28" t="s">
+      <c r="E139" s="28" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="16">
+    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A140" s="16">
         <v>40132</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B140" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C140" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E139" s="28" t="s">
+      <c r="E140" s="28" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="16">
+    <row r="141" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="16">
         <v>40133</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C141" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E140" s="28" t="s">
+      <c r="E141" s="28" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="16">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" s="16">
         <v>40135</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B142" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C142" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E141" s="28" t="s">
+      <c r="E142" s="28" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="16">
+    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A143" s="16">
         <v>40134</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B143" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C143" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E142" s="28" t="s">
+      <c r="E143" s="28" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="16">
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A144" s="16">
         <v>40131</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C144" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="E143" s="28" t="s">
+      <c r="E144" s="28" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="16">
+    <row r="145" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A145" s="16">
         <v>40137</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="E144" s="29" t="s">
+      <c r="E145" s="29" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="16">
+    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A146" s="16">
         <v>40136</v>
       </c>
-      <c r="B145" s="8" t="s">
+      <c r="B146" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C146" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="E145" s="28" t="s">
+      <c r="E146" s="28" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="16">
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A147" s="16">
         <v>40138</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C147" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="E146" s="28" t="s">
+      <c r="E147" s="28" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="16">
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A148" s="16">
         <v>40141</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C148" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="E147" s="29" t="s">
+      <c r="E148" s="29" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" s="16">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="16">
         <v>40129</v>
       </c>
-      <c r="B148" s="19" t="s">
+      <c r="B149" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C149" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D148" s="16" t="s">
+      <c r="D149" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E148" s="28" t="s">
+      <c r="E149" s="28" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B149" s="25" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B150" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C150" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="E149" s="28" t="s">
+      <c r="E150" s="28" t="s">
         <v>375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dose Forms: Changed intraocular injection to irrigation
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\OneDrive\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_BC82D73D065B19057060F70E5976D2E92A5E43EC" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BFAD4AF6-EC3B-4FE8-8B55-68FBF37FC66C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4404"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1611,19 +1617,19 @@
     <t>poudre pour pulvérisation cutanée</t>
   </si>
   <si>
-    <t>powder for solution for intraocular injection</t>
-  </si>
-  <si>
     <t>Solid sterile preparation consisting of one or more powders, including freeze-dried powders, intended to be dissolved in the specified liquid to obtain a solution for intraocular irrigation.</t>
   </si>
   <si>
     <t>Poudre pour solution pour irrigation intraoculaire</t>
+  </si>
+  <si>
+    <t>powder for solution for intraocular irrigation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2079,27 +2085,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.21875" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="54.5546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5234375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.20703125" customWidth="1"/>
+    <col min="4" max="4" width="27.89453125" customWidth="1"/>
+    <col min="5" max="5" width="54.5234375" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2119,7 +2125,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16">
         <v>40007</v>
       </c>
@@ -2148,7 +2154,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="16">
         <v>40079</v>
       </c>
@@ -2165,7 +2171,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="16">
         <v>40108</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="16">
         <v>40111</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="16">
         <v>40107</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="16">
         <v>40112</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="16">
         <v>40113</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="16">
         <v>40116</v>
       </c>
@@ -2263,7 +2269,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="16">
         <v>40118</v>
       </c>
@@ -2278,7 +2284,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="16">
         <v>40119</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="16">
         <v>40121</v>
       </c>
@@ -2308,7 +2314,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="16">
         <v>40124</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="16">
         <v>40106</v>
       </c>
@@ -2340,7 +2346,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="17" t="s">
         <v>478</v>
       </c>
@@ -2354,7 +2360,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="16">
         <v>40126</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="16">
         <v>40084</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="16">
         <v>40082</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="16">
         <v>40142</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="20">
         <v>40037</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20">
         <v>40048</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="20">
         <v>40071</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20">
         <v>40081</v>
       </c>
@@ -2587,7 +2593,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="16">
         <v>40069</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="16">
         <v>40068</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="16">
         <v>40022</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16">
         <v>40027</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="16">
         <v>40038</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="16">
         <v>40041</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="16">
         <v>40042</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="16">
         <v>40130</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="16">
         <v>40023</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="16">
         <v>40061</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="16">
         <v>40080</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="16">
         <v>40046</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="16">
         <v>40047</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="16">
         <v>40031</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="16">
         <v>40028</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="16">
         <v>40057</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="16">
         <v>40065</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="16">
         <v>40075</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="16">
         <v>40078</v>
       </c>
@@ -3383,7 +3389,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="16">
         <v>40076</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="16">
         <v>40009</v>
       </c>
@@ -3456,7 +3462,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="16">
         <v>40089</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="16">
         <v>40090</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="16">
         <v>40117</v>
       </c>
@@ -3558,7 +3564,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="16">
         <v>40102</v>
       </c>
@@ -3588,7 +3594,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="16">
         <v>40120</v>
       </c>
@@ -3605,7 +3611,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="16">
         <v>40014</v>
       </c>
@@ -3620,7 +3626,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="16">
         <v>40122</v>
       </c>
@@ -3635,7 +3641,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="16">
         <v>40040</v>
       </c>
@@ -3650,7 +3656,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="16">
         <v>40026</v>
       </c>
@@ -3725,7 +3731,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" s="17" t="s">
         <v>475</v>
       </c>
@@ -3739,7 +3745,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="16">
         <v>40018</v>
       </c>
@@ -3769,7 +3775,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="16">
         <v>40017</v>
       </c>
@@ -3784,19 +3790,19 @@
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="21"/>
       <c r="B109" s="17" t="s">
+        <v>484</v>
+      </c>
+      <c r="C109" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="E109" s="28" t="s">
         <v>483</v>
       </c>
-      <c r="E109" s="28" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="16">
         <v>40039</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="16">
         <v>40021</v>
       </c>
@@ -3843,7 +3849,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="16">
         <v>40055</v>
       </c>
@@ -3858,7 +3864,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="16">
         <v>40062</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="16">
         <v>40083</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="16">
         <v>40103</v>
       </c>
@@ -3905,7 +3911,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" s="17" t="s">
         <v>474</v>
       </c>
@@ -3917,7 +3923,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="16">
         <v>40020</v>
       </c>
@@ -3932,7 +3938,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="16">
         <v>40099</v>
       </c>
@@ -3947,7 +3953,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="16">
         <v>40091</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="16">
         <v>40093</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="16">
         <v>40092</v>
       </c>
@@ -3994,7 +4000,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="16">
         <v>40095</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="16">
         <v>40094</v>
       </c>
@@ -4022,7 +4028,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="16">
         <v>40098</v>
       </c>
@@ -4036,7 +4042,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="22">
         <v>40140</v>
       </c>
@@ -4048,7 +4054,7 @@
       </c>
       <c r="E126" s="28"/>
     </row>
-    <row r="127" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="16">
         <v>40123</v>
       </c>
@@ -4062,7 +4068,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="16">
         <v>40032</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="16">
         <v>40013</v>
       </c>
@@ -4090,7 +4096,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="16">
         <v>40001</v>
       </c>
@@ -4104,7 +4110,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="16">
         <v>40036</v>
       </c>
@@ -4118,7 +4124,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="16">
         <v>40104</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="16">
         <v>40105</v>
       </c>
@@ -4146,7 +4152,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="16">
         <v>40097</v>
       </c>
@@ -4160,7 +4166,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="16">
         <v>40019</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="16">
         <v>40128</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="22">
         <v>40077</v>
       </c>
@@ -4208,7 +4214,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="16">
         <v>40100</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="16">
         <v>40012</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="16">
         <v>40132</v>
       </c>
@@ -4250,7 +4256,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="16">
         <v>40133</v>
       </c>
@@ -4264,7 +4270,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="16">
         <v>40135</v>
       </c>
@@ -4278,7 +4284,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="16">
         <v>40134</v>
       </c>
@@ -4292,7 +4298,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="16">
         <v>40131</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="16">
         <v>40137</v>
       </c>
@@ -4320,7 +4326,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="16">
         <v>40136</v>
       </c>
@@ -4334,7 +4340,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="16">
         <v>40138</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="16">
         <v>40141</v>
       </c>
@@ -4362,7 +4368,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="16">
         <v>40129</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B150" s="25" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
Added oral/rectal suspension to CCDD dosage form concepts
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\OneDrive\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_BC82D73D065B19057060F70E5976D2E92A5E43EC" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BFAD4AF6-EC3B-4FE8-8B55-68FBF37FC66C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="4404"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$152</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="488">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1625,11 +1619,33 @@
   <si>
     <t>powder for solution for intraocular irrigation</t>
   </si>
+  <si>
+    <t>oral/rectal suspension</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Liquid preparation consisting of a suspension intended for oral or rectal use. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This term is only to be used in cases where there is not a single predominant route of administration for the medicinal product.</t>
+    </r>
+  </si>
+  <si>
+    <t>Suspension buvable/rectale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2085,27 +2101,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E150"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5234375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.20703125" customWidth="1"/>
-    <col min="4" max="4" width="27.89453125" customWidth="1"/>
-    <col min="5" max="5" width="54.5234375" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2125,7 +2141,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>40007</v>
       </c>
@@ -2154,7 +2170,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>40079</v>
       </c>
@@ -2171,7 +2187,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>40108</v>
       </c>
@@ -2188,7 +2204,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>40111</v>
       </c>
@@ -2203,7 +2219,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>40107</v>
       </c>
@@ -2218,7 +2234,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>40112</v>
       </c>
@@ -2235,7 +2251,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>40113</v>
       </c>
@@ -2252,7 +2268,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>40116</v>
       </c>
@@ -2269,7 +2285,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>40118</v>
       </c>
@@ -2284,7 +2300,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>40119</v>
       </c>
@@ -2299,7 +2315,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>40121</v>
       </c>
@@ -2314,7 +2330,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>40124</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>40106</v>
       </c>
@@ -2346,7 +2362,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>478</v>
       </c>
@@ -2360,7 +2376,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>40126</v>
       </c>
@@ -2418,7 +2434,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>40084</v>
       </c>
@@ -2450,7 +2466,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>40082</v>
       </c>
@@ -2467,7 +2483,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>40142</v>
       </c>
@@ -2512,7 +2528,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>40037</v>
       </c>
@@ -2544,7 +2560,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>40048</v>
       </c>
@@ -2561,7 +2577,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>40071</v>
       </c>
@@ -2576,7 +2592,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>40081</v>
       </c>
@@ -2593,7 +2609,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>40069</v>
       </c>
@@ -2608,7 +2624,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>40068</v>
       </c>
@@ -2653,7 +2669,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>40022</v>
       </c>
@@ -2668,7 +2684,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>40027</v>
       </c>
@@ -2713,7 +2729,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>40038</v>
       </c>
@@ -2728,7 +2744,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>40041</v>
       </c>
@@ -2743,7 +2759,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>40042</v>
       </c>
@@ -2836,7 +2852,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>40130</v>
       </c>
@@ -2851,7 +2867,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>40023</v>
       </c>
@@ -2868,7 +2884,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>40061</v>
       </c>
@@ -2885,7 +2901,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>40080</v>
       </c>
@@ -2917,7 +2933,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>40046</v>
       </c>
@@ -3011,7 +3027,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>40047</v>
       </c>
@@ -3026,7 +3042,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>40031</v>
       </c>
@@ -3041,7 +3057,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>40028</v>
       </c>
@@ -3056,7 +3072,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>40057</v>
       </c>
@@ -3252,7 +3268,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="16">
         <v>40065</v>
       </c>
@@ -3297,7 +3313,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="16">
         <v>40075</v>
       </c>
@@ -3357,7 +3373,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="16">
         <v>40078</v>
       </c>
@@ -3374,1025 +3390,1037 @@
         <v>443</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="16">
+    <row r="82" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B82" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="28" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="16">
         <v>40066</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C83" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="D82" s="1"/>
-      <c r="E82" s="28" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="16">
-        <v>40076</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="28" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="16">
-        <v>40002</v>
+        <v>40076</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>167</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="16">
-        <v>40009</v>
+        <v>40002</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="16">
+        <v>40009</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="16">
+    <row r="87" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="16">
         <v>40008</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B87" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C87" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="E86" s="28" t="s">
+      <c r="E87" s="28" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="16">
+    <row r="88" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="16">
         <v>40005</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C87" s="18" t="s">
+      <c r="C88" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="D88" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="16">
+    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="16">
         <v>40089</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C89" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E88" s="28" t="s">
+      <c r="E89" s="28" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="16">
+    <row r="90" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="16">
         <v>40086</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C90" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E89" s="28" t="s">
+      <c r="E90" s="28" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="16">
+    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="16">
         <v>40087</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B91" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C91" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E90" s="28" t="s">
+      <c r="E91" s="28" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="16">
+    <row r="92" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="16">
         <v>40088</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C92" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E91" s="29" t="s">
+      <c r="E92" s="29" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="16">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="16">
         <v>40090</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C93" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E92" s="28" t="s">
+      <c r="E93" s="28" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="16">
+    <row r="94" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="16">
         <v>40117</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B94" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D94" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="E93" s="28" t="s">
+      <c r="E94" s="28" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="16">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="16">
         <v>40102</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B95" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C95" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="D94" s="1"/>
-      <c r="E94" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="16">
-        <v>40139</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="28" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="16">
+        <v>40139</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="28" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="16">
+    <row r="97" spans="1:5" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="16">
         <v>40120</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B97" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C97" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D97" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="E96" s="28" t="s">
+      <c r="E97" s="28" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="16">
+    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="16">
         <v>40014</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="29" t="s">
+      <c r="D98" s="1"/>
+      <c r="E98" s="29" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="16">
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A99" s="16">
         <v>40122</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C99" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="28" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="16">
-        <v>40040</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="28" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="16">
-        <v>40026</v>
+        <v>40040</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="16">
+        <v>40026</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="28" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="16">
+    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="16">
         <v>40054</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C102" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D102" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E101" s="28" t="s">
+      <c r="E102" s="28" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="16">
+    <row r="103" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="16">
         <v>40049</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C103" s="11" t="s">
         <v>293</v>
-      </c>
-      <c r="D102" s="1"/>
-      <c r="E102" s="29" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="21"/>
-      <c r="B103" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>292</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="29" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="21"/>
+      <c r="B104" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="29" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="16">
+    <row r="105" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="16">
         <v>40085</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C105" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="28" t="s">
+      <c r="D105" s="1"/>
+      <c r="E105" s="28" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B105" s="17" t="s">
+    <row r="106" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B106" s="17" t="s">
         <v>475</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C106" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="D105" s="11" t="s">
+      <c r="D106" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="E105" s="28" t="s">
+      <c r="E106" s="28" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="16">
+    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="16">
         <v>40018</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C107" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="28" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="16">
-        <v>40096</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="16">
-        <v>40017</v>
+        <v>40096</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="28" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="16">
+        <v>40017</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="28" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="21"/>
-      <c r="B109" s="17" t="s">
+    <row r="110" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="21"/>
+      <c r="B110" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C110" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="E109" s="28" t="s">
+      <c r="E110" s="28" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="16">
+    <row r="111" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="16">
         <v>40039</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C111" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D110" s="11" t="s">
+      <c r="D111" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E110" s="28" t="s">
+      <c r="E111" s="28" t="s">
         <v>400</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="16">
-        <v>40016</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C111" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="28" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="16">
-        <v>40021</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="16">
-        <v>40055</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>306</v>
+        <v>40021</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="28" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="16">
-        <v>40062</v>
+        <v>40055</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="28" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="16">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="28" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="16">
+        <v>40083</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="28" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="16">
+    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A117" s="16">
         <v>40103</v>
       </c>
-      <c r="B116" s="15" t="s">
+      <c r="B117" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C117" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D117" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E116" s="29" t="s">
+      <c r="E117" s="29" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B117" s="17" t="s">
+    <row r="118" spans="1:5" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B118" s="17" t="s">
         <v>474</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C118" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="D117" s="5"/>
-      <c r="E117" s="29" t="s">
+      <c r="D118" s="5"/>
+      <c r="E118" s="29" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="16">
+    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A119" s="16">
         <v>40020</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C119" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D118" s="1"/>
-      <c r="E118" s="29" t="s">
+      <c r="D119" s="1"/>
+      <c r="E119" s="29" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="16">
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="16">
         <v>40099</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C120" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="D119" s="1"/>
-      <c r="E119" s="28" t="s">
+      <c r="D120" s="1"/>
+      <c r="E120" s="28" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="16">
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" s="16">
         <v>40091</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C121" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D120" s="1"/>
-      <c r="E120" s="29" t="s">
+      <c r="D121" s="1"/>
+      <c r="E121" s="29" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="16">
+    <row r="122" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="16">
         <v>40093</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="B122" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C122" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D121" s="11"/>
-      <c r="E121" s="29" t="s">
+      <c r="D122" s="11"/>
+      <c r="E122" s="29" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="16">
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A123" s="16">
         <v>40092</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C123" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="D122" s="11" t="s">
+      <c r="D123" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E122" s="28" t="s">
+      <c r="E123" s="28" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="16">
+    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A124" s="16">
         <v>40095</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C124" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E123" s="28" t="s">
+      <c r="E124" s="28" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="16">
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="16">
         <v>40094</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C125" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E124" s="29" t="s">
+      <c r="E125" s="29" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="16">
+    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A126" s="16">
         <v>40098</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C126" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E125" s="29" t="s">
+      <c r="E126" s="29" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="22">
+    <row r="127" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="22">
         <v>40140</v>
       </c>
-      <c r="B126" s="23" t="s">
+      <c r="B127" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="C126" s="24" t="s">
+      <c r="C127" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="E126" s="28"/>
-    </row>
-    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="16">
+      <c r="E127" s="28"/>
+    </row>
+    <row r="128" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A128" s="16">
         <v>40123</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C128" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="E127" s="28" t="s">
+      <c r="E128" s="28" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="16">
+    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A129" s="16">
         <v>40032</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C129" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E128" s="28" t="s">
+      <c r="E129" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="16">
+    <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A130" s="16">
         <v>40013</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C129" s="11" t="s">
+      <c r="C130" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="E129" s="28" t="s">
+      <c r="E130" s="28" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="16">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="16">
         <v>40001</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C131" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E130" s="28" t="s">
+      <c r="E131" s="28" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="16">
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A132" s="16">
         <v>40036</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C131" s="11" t="s">
+      <c r="C132" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E131" s="28" t="s">
+      <c r="E132" s="28" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="16">
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A133" s="16">
         <v>40104</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C133" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E132" s="28" t="s">
+      <c r="E133" s="28" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="16">
+    <row r="134" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A134" s="16">
         <v>40105</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C134" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E133" s="28" t="s">
+      <c r="E134" s="28" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="16">
+    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A135" s="16">
         <v>40097</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C135" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E134" s="28" t="s">
+      <c r="E135" s="28" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="16">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" s="16">
         <v>40019</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C136" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E135" s="28" t="s">
+      <c r="E136" s="28" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="16">
+    <row r="137" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="16">
         <v>40128</v>
       </c>
-      <c r="B136" s="19" t="s">
+      <c r="B137" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C137" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D136" s="16" t="s">
+      <c r="D137" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E136" s="28" t="s">
+      <c r="E137" s="28" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="22">
+    <row r="138" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A138" s="22">
         <v>40077</v>
       </c>
-      <c r="B137" s="25" t="s">
+      <c r="B138" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C137" s="24" t="s">
+      <c r="C138" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="D137" s="22" t="s">
+      <c r="D138" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="E137" s="31" t="s">
+      <c r="E138" s="31" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="16">
+    <row r="139" spans="1:5" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A139" s="16">
         <v>40100</v>
       </c>
-      <c r="B138" s="17" t="s">
+      <c r="B139" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C139" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="E138" s="28" t="s">
+      <c r="E139" s="28" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="16">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" s="16">
         <v>40012</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C140" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E139" s="28" t="s">
+      <c r="E140" s="28" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="16">
+    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A141" s="16">
         <v>40132</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B141" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C141" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E140" s="28" t="s">
+      <c r="E141" s="28" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="16">
+    <row r="142" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="16">
         <v>40133</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C142" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E141" s="28" t="s">
+      <c r="E142" s="28" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="16">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="16">
         <v>40135</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B143" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C143" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E142" s="28" t="s">
+      <c r="E143" s="28" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="16">
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A144" s="16">
         <v>40134</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B144" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C144" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E143" s="28" t="s">
+      <c r="E144" s="28" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="16">
+    <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A145" s="16">
         <v>40131</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="E144" s="28" t="s">
+      <c r="E145" s="28" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="16">
+    <row r="146" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A146" s="16">
         <v>40137</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C146" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="E145" s="29" t="s">
+      <c r="E146" s="29" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="16">
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A147" s="16">
         <v>40136</v>
       </c>
-      <c r="B146" s="8" t="s">
+      <c r="B147" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C147" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="E146" s="28" t="s">
+      <c r="E147" s="28" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="16">
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A148" s="16">
         <v>40138</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C148" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="E147" s="28" t="s">
+      <c r="E148" s="28" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" s="16">
+    <row r="149" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A149" s="16">
         <v>40141</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C149" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="E148" s="29" t="s">
+      <c r="E149" s="29" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="16">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="16">
         <v>40129</v>
       </c>
-      <c r="B149" s="19" t="s">
+      <c r="B150" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C150" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D149" s="16" t="s">
+      <c r="D150" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E149" s="28" t="s">
+      <c r="E150" s="28" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B150" s="25" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B151" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="C151" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="E150" s="28" t="s">
+      <c r="E151" s="28" t="s">
         <v>375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dose forms: added mucosal gel
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\OneDrive\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_BD82D73D065B19C571EAE2819C72FF3612D96FE6" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F9B29B11-B2B4-485D-979A-B8736F900997}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E1660-3B9A-48D7-98EE-992931DDB55A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$154</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="496">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1143,9 +1143,6 @@
   </si>
   <si>
     <t xml:space="preserve">solution pour application cutanée </t>
-  </si>
-  <si>
-    <t>pulvérisation cutanée</t>
   </si>
   <si>
     <t xml:space="preserve">  
@@ -1276,9 +1273,6 @@
     <t>comprimé sublingual</t>
   </si>
   <si>
-    <t>solution pour pulvérisation sublinguale</t>
-  </si>
-  <si>
     <t>solution pour dialyse péritonéale</t>
   </si>
   <si>
@@ -1543,9 +1537,6 @@
   </si>
   <si>
     <t>EDQM</t>
-  </si>
-  <si>
-    <t>poudre pour pulvérisation cutanée</t>
   </si>
   <si>
     <t>Solid sterile preparation consisting of one or more powders, including freeze-dried powders, intended to be dissolved in the specified liquid to obtain a solution for intraocular irrigation.</t>
@@ -1658,6 +1649,27 @@
   </si>
   <si>
     <t>suspension orale/rectale</t>
+  </si>
+  <si>
+    <t>mucosal gel</t>
+  </si>
+  <si>
+    <t>Semi-solid single-dose or multidose preparation consisting of a hydrophilic gel intended for mucosal use. It is applied to any mucosal surface to obtain a local effect.  Specific mucosal use sites are excluded (e.g. urethral gel, oromucosal gel)</t>
+  </si>
+  <si>
+    <t>Not present in EDQM.</t>
+  </si>
+  <si>
+    <t>gel muqueux</t>
+  </si>
+  <si>
+    <t>solution pour vaporisation sublinguale</t>
+  </si>
+  <si>
+    <t>vaporisation cutanée</t>
+  </si>
+  <si>
+    <t>poudre pour vaporisation cutanée</t>
   </si>
 </sst>
 </file>
@@ -2114,11 +2126,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2288,7 +2300,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>40118</v>
       </c>
@@ -2313,7 +2325,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2330,7 +2342,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>40124</v>
       </c>
@@ -2358,21 +2370,21 @@
         <v>33</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>336</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>458</v>
-      </c>
       <c r="E16" s="20" t="s">
-        <v>459</v>
+        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2387,7 +2399,7 @@
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2413,7 +2425,7 @@
         <v>39</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2427,7 +2439,7 @@
         <v>41</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2444,7 +2456,7 @@
         <v>163</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2455,14 +2467,14 @@
         <v>44</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="21" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>40082</v>
       </c>
@@ -2476,7 +2488,7 @@
         <v>163</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2490,7 +2502,7 @@
         <v>48</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2504,7 +2516,7 @@
         <v>50</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2518,7 +2530,7 @@
         <v>52</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2535,7 +2547,7 @@
         <v>55</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2549,7 +2561,7 @@
         <v>57</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2566,7 +2578,7 @@
         <v>60</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2580,7 +2592,7 @@
         <v>62</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2597,7 +2609,7 @@
         <v>60</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2611,7 +2623,7 @@
         <v>66</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2625,7 +2637,7 @@
         <v>68</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2653,7 +2665,7 @@
         <v>72</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2668,10 +2680,10 @@
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="19" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>40027</v>
       </c>
@@ -2682,7 +2694,7 @@
         <v>76</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2696,21 +2708,21 @@
         <v>78</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="E39" s="19" t="s">
         <v>487</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2724,10 +2736,10 @@
         <v>80</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>40038</v>
       </c>
@@ -2738,10 +2750,10 @@
         <v>82</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>40041</v>
       </c>
@@ -2752,10 +2764,10 @@
         <v>84</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>40042</v>
       </c>
@@ -2769,7 +2781,7 @@
         <v>87</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2783,7 +2795,7 @@
         <v>89</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2794,7 +2806,7 @@
         <v>303</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2811,7 +2823,7 @@
         <v>319</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2842,7 +2854,7 @@
         <v>95</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2856,7 +2868,7 @@
         <v>97</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -2873,7 +2885,7 @@
         <v>100</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -2890,10 +2902,10 @@
         <v>102</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>40080</v>
       </c>
@@ -2907,7 +2919,7 @@
         <v>102</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2921,900 +2933,900 @@
         <v>105</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54">
+      <c r="B54" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
         <v>40046</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E54" s="19" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55">
+      <c r="E55" s="19" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
         <v>40043</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="19" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56">
-        <v>40044</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="E56" s="19" t="s">
-        <v>415</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
-        <v>40045</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>113</v>
+        <v>40044</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
+        <v>40045</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
         <v>40030</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="19" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59">
+      <c r="E59" s="19" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
         <v>40029</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D60" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E59" s="19" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60">
+      <c r="E60" s="19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
         <v>40047</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="19" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61">
-        <v>40031</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>123</v>
-      </c>
       <c r="E61" s="19" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
+        <v>40031</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
         <v>40028</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E62" s="19" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63">
-        <v>40057</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" t="s">
-        <v>128</v>
-      </c>
       <c r="E63" s="19" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
+        <v>40057</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
         <v>40050</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="19" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65">
+      <c r="E65" s="19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
         <v>40051</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E66" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>40052</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>40053</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" s="19" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66">
-        <v>40052</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E66" s="20" t="s">
+    <row r="69" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>40056</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E69" s="20" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67">
-        <v>40053</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D67" t="s">
-        <v>139</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68">
-        <v>40056</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69">
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
         <v>40058</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D70" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="E69" s="19" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70">
+      <c r="E70" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
         <v>40059</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>290</v>
       </c>
-      <c r="E70" s="20" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71">
-        <v>40060</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>431</v>
+      <c r="E71" s="20" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
-        <v>40063</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>145</v>
+        <v>40060</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E72" s="19" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
-        <v>40144</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>454</v>
+        <v>40063</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D73" s="7"/>
+        <v>320</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="E73" s="19" t="s">
-        <v>469</v>
+        <v>427</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
+        <v>40144</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D74" s="7"/>
+      <c r="E74" s="19" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
         <v>40145</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="C74" s="7" t="s">
+      <c r="B75" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D74" s="7"/>
-      <c r="E74" s="20" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75">
-        <v>40065</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>471</v>
+      <c r="D75" s="7"/>
+      <c r="E75" s="20" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
-        <v>40067</v>
+        <v>40065</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>343</v>
+        <v>468</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
+        <v>40067</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
         <v>40072</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C78" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E77" s="19" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78">
-        <v>40075</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E78" s="20" t="s">
-        <v>409</v>
+      <c r="E78" s="19" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
+        <v>40075</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E79" s="20" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
         <v>40074</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E79" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80">
-        <v>40064</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="E80" s="19" t="s">
-        <v>472</v>
+        <v>408</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
+        <v>40064</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
         <v>40070</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E81" s="19" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82">
+      <c r="E82" s="19" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
         <v>40078</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C83" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D83" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E82" s="19" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B83" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="D83" s="7"/>
       <c r="E83" s="19" t="s">
-        <v>491</v>
+        <v>426</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84">
-        <v>40066</v>
-      </c>
       <c r="B84" s="3" t="s">
-        <v>164</v>
+        <v>460</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>461</v>
+      </c>
+      <c r="D84" s="7"/>
       <c r="E84" s="19" t="s">
-        <v>432</v>
+        <v>488</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
-        <v>40076</v>
+        <v>40066</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
-        <v>40002</v>
+        <v>40076</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
+        <v>40002</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
         <v>40009</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C88" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E87" s="19" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88">
+      <c r="E88" s="19" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
         <v>40008</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C89" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="E88" s="19" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89">
+      <c r="E89" s="19" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
         <v>40005</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D90" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90">
+    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
         <v>40089</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>177</v>
       </c>
-      <c r="E90" s="19" t="s">
+      <c r="E91" s="19" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>40086</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>40087</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D93" t="s">
+        <v>183</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>40088</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D94" t="s">
+        <v>186</v>
+      </c>
+      <c r="E94" s="20" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91">
-        <v>40086</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92">
-        <v>40087</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D92" t="s">
-        <v>183</v>
-      </c>
-      <c r="E92" s="19" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93">
-        <v>40088</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" t="s">
-        <v>186</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94">
-        <v>40090</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D94" t="s">
-        <v>189</v>
-      </c>
-      <c r="E94" s="19" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
+        <v>40090</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D95" t="s">
+        <v>189</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
         <v>40117</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B96" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C96" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D96" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="E95" s="19" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96">
+      <c r="E96" s="19" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
         <v>40102</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B97" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C97" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E97" s="19" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>40139</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E98" s="19" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>40120</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E99" s="19" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97">
-        <v>40139</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E97" s="19" t="s">
+    <row r="100" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>40014</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E100" s="20" t="s">
         <v>438</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98">
-        <v>40120</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E98" s="19" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99">
-        <v>40014</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E99" s="20" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100">
-        <v>40122</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E100" s="19" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
-        <v>40040</v>
+        <v>40122</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
-        <v>40026</v>
+        <v>40040</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
+        <v>40026</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E103" s="19" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
         <v>40054</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C104" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D104" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E103" s="19" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104">
+      <c r="E104" s="19" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
         <v>40049</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C105" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E104" s="20" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="12"/>
-      <c r="B105" s="3" t="s">
+      <c r="E105" s="20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="12"/>
+      <c r="B106" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C106" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="E105" s="20" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106">
+      <c r="E106" s="20" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
         <v>40085</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="E106" s="19" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B107" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="C107" s="7" t="s">
+      <c r="E107" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B108" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="E108" s="19" t="s">
         <v>449</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="E107" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108">
-        <v>40018</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E108" s="19" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
-        <v>40096</v>
+        <v>40018</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
+        <v>40096</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E110" s="19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
         <v>40017</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C111" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="E110" s="19" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="12"/>
-      <c r="B111" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>460</v>
-      </c>
       <c r="E111" s="19" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="12"/>
+      <c r="B112" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
         <v>40039</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C113" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D113" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="E112" s="19" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113">
-        <v>40016</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="E113" s="19" t="s">
         <v>391</v>
@@ -3822,337 +3834,337 @@
     </row>
     <row r="114" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114">
-        <v>40021</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
+        <v>40021</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E115" s="19" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
         <v>40055</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C116" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E115" s="19" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116">
-        <v>40062</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>223</v>
-      </c>
       <c r="E116" s="19" t="s">
-        <v>389</v>
+        <v>474</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A117">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E117" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
+        <v>40083</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E118" s="19" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
         <v>40103</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C119" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D119" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E118" s="20" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B119" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="D119" s="4"/>
       <c r="E119" s="20" t="s">
-        <v>448</v>
+        <v>385</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120">
+      <c r="B120" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D120" s="4"/>
+      <c r="E120" s="20" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
         <v>40020</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C121" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E120" s="20" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121">
+      <c r="E121" s="20" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
         <v>40099</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C122" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E121" s="19" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122">
-        <v>40091</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E122" s="20" t="s">
-        <v>384</v>
+      <c r="E122" s="19" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A123">
+        <v>40091</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E123" s="20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124">
         <v>40093</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B124" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="C124" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D123" s="7"/>
-      <c r="E123" s="20" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124">
-        <v>40092</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="E124" s="19" t="s">
-        <v>383</v>
+      <c r="D124" s="7"/>
+      <c r="E124" s="20" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125">
+        <v>40092</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="E125" s="19" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126">
         <v>40095</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B126" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C126" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E125" s="19" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126">
-        <v>40094</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="E126" s="20" t="s">
-        <v>378</v>
+      <c r="E126" s="19" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A127">
+        <v>40094</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E127" s="20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128">
         <v>40098</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B128" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="C128" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="E127" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="13">
+      <c r="E128" s="20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="13">
         <v>40140</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="B129" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="C128" s="15" t="s">
+      <c r="C129" s="15" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129">
+    <row r="130" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130">
         <v>40123</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B130" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C129" s="7" t="s">
+      <c r="C130" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E129" s="19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130">
-        <v>40032</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>247</v>
-      </c>
       <c r="E130" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131">
+        <v>40032</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E131" s="19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132">
         <v>40013</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B132" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C132" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E131" s="19" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132">
+      <c r="E132" s="19" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133">
         <v>40001</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B133" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C132" s="7" t="s">
+      <c r="C133" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E132" s="19" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133">
+      <c r="E133" s="19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134">
         <v>40036</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B134" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C134" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E133" s="19" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134">
+      <c r="E134" s="19" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135">
         <v>40104</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B135" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C135" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E134" s="19" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135">
+      <c r="E135" s="19" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136">
         <v>40105</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B136" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C136" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E135" s="19" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136">
+      <c r="E136" s="19" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137">
         <v>40097</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B137" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C137" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="E136" s="19" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137">
-        <v>40019</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="E137" s="19" t="s">
         <v>364</v>
@@ -4160,117 +4172,117 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A138">
+        <v>40019</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E138" s="19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139">
         <v>40128</v>
       </c>
-      <c r="B138" s="11" t="s">
+      <c r="B139" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="C138" s="7" t="s">
+      <c r="C139" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D139" t="s">
         <v>313</v>
       </c>
-      <c r="E138" s="19" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="13">
+      <c r="E139" s="19" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="13">
         <v>40077</v>
       </c>
-      <c r="B139" s="16" t="s">
+      <c r="B140" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C140" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D139" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="E139" s="22" t="s">
+      <c r="D140" s="13" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140">
+      <c r="E140" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141">
         <v>40100</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B141" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C140" s="7" t="s">
+      <c r="C141" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="E140" s="19" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141">
-        <v>40012</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="E141" s="19" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A142">
-        <v>40132</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>266</v>
+        <v>40012</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E142" s="19" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A143">
+        <v>40132</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E143" s="19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144">
         <v>40133</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B144" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C144" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="E143" s="19" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144">
+      <c r="E144" s="19" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145">
         <v>40135</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="B145" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C144" s="7" t="s">
+      <c r="C145" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="E144" s="19" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145">
-        <v>40134</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="E145" s="19" t="s">
         <v>357</v>
@@ -4278,100 +4290,114 @@
     </row>
     <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146">
-        <v>40131</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>274</v>
+        <v>40134</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>272</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E146" s="19" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
+        <v>40131</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E147" s="19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148">
         <v>40137</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C147" s="7" t="s">
+      <c r="C148" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="E147" s="20" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148">
-        <v>40136</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="E148" s="19" t="s">
+      <c r="E148" s="20" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A149">
-        <v>40138</v>
+        <v>40136</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E149" s="19" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
+        <v>40138</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E150" s="19" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151">
         <v>40141</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B151" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C150" s="7" t="s">
+      <c r="C151" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="E150" s="20" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A151">
+      <c r="E151" s="20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152">
         <v>40129</v>
       </c>
-      <c r="B151" s="11" t="s">
+      <c r="B152" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="C151" s="7" t="s">
+      <c r="C152" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D152" t="s">
         <v>313</v>
       </c>
-      <c r="E151" s="19" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B152" s="16" t="s">
+      <c r="E152" s="19" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B153" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C153" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="C152" s="7" t="s">
+      <c r="E153" s="19" t="s">
         <v>368</v>
-      </c>
-      <c r="E152" s="19" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dose Forms: Added oromucosal/laryngopharyngeal solution
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\OneDrive\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E1660-3B9A-48D7-98EE-992931DDB55A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B718EBE7-AEFA-44DA-87A9-F2FEFCDDF7EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$155</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="499">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -1671,12 +1671,21 @@
   <si>
     <t>poudre pour vaporisation cutanée</t>
   </si>
+  <si>
+    <t>oromucosal/laryngopharyngeal solution</t>
+  </si>
+  <si>
+    <t>Liquid preparation consisting of a solution intended for oromucosal or laryngopharyngeal use.</t>
+  </si>
+  <si>
+    <t>solution buccale/laryngopharyngée</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1753,6 +1762,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1804,7 +1820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1846,6 +1862,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2126,11 +2143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3487,916 +3504,928 @@
         <v>174</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="23" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
         <v>40089</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>177</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E92" s="19" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92">
+    <row r="93" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
         <v>40086</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C93" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D93" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E93" s="19" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93">
+    <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
         <v>40087</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B94" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C94" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>183</v>
       </c>
-      <c r="E93" s="19" t="s">
+      <c r="E94" s="19" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94">
+    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
         <v>40088</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C95" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>186</v>
       </c>
-      <c r="E94" s="20" t="s">
+      <c r="E95" s="20" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95">
-        <v>40090</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D95" t="s">
-        <v>189</v>
-      </c>
-      <c r="E95" s="19" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
+        <v>40090</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D96" t="s">
+        <v>189</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
         <v>40117</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B97" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C97" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D97" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E97" s="19" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
         <v>40102</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B98" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E97" s="19" t="s">
+      <c r="E98" s="19" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98">
+    <row r="99" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
         <v>40139</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E99" s="19" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99">
+    <row r="100" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
         <v>40120</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B100" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C100" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D100" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E100" s="19" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100">
+    <row r="101" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
         <v>40014</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C101" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E100" s="20" t="s">
+      <c r="E101" s="20" t="s">
         <v>438</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101">
-        <v>40122</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E101" s="19" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
-        <v>40040</v>
+        <v>40122</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
-        <v>40026</v>
+        <v>40040</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
+        <v>40026</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
         <v>40054</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C105" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D105" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E104" s="19" t="s">
+      <c r="E105" s="19" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105">
+    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
         <v>40049</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C106" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E105" s="20" t="s">
+      <c r="E106" s="20" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="12"/>
-      <c r="B106" s="3" t="s">
+    <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="12"/>
+      <c r="B107" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="E106" s="20" t="s">
+      <c r="E107" s="20" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107">
+    <row r="108" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
         <v>40085</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="E107" s="19" t="s">
+      <c r="E108" s="19" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B108" s="3" t="s">
+    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B109" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="D109" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="E108" s="19" t="s">
+      <c r="E109" s="19" t="s">
         <v>449</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109">
-        <v>40018</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E109" s="19" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
-        <v>40096</v>
+        <v>40018</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E110" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
+        <v>40096</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
         <v>40017</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="E111" s="19" t="s">
+      <c r="E112" s="19" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="12"/>
-      <c r="B112" s="3" t="s">
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="12"/>
+      <c r="B113" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C113" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E113" s="19" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113">
+    <row r="114" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
         <v>40039</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D114" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E113" s="19" t="s">
+      <c r="E114" s="19" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114">
-        <v>40016</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E114" s="19" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
-        <v>40021</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>220</v>
+        <v>40016</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116">
+        <v>40021</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
         <v>40055</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E117" s="19" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117">
-        <v>40062</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
-        <v>40083</v>
+        <v>40062</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E118" s="19" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A119">
+        <v>40083</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E119" s="19" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
         <v>40103</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C120" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D120" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E119" s="20" t="s">
+      <c r="E120" s="20" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B120" s="3" t="s">
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B121" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C121" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="D120" s="4"/>
-      <c r="E120" s="20" t="s">
+      <c r="D121" s="4"/>
+      <c r="E121" s="20" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121">
+    <row r="122" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
         <v>40020</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C122" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E121" s="20" t="s">
+      <c r="E122" s="20" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122">
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123">
         <v>40099</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C123" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E122" s="19" t="s">
+      <c r="E123" s="19" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123">
-        <v>40091</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E123" s="20" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A124">
+        <v>40091</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E124" s="20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125">
         <v>40093</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B125" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="C125" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D124" s="7"/>
-      <c r="E124" s="20" t="s">
+      <c r="D125" s="7"/>
+      <c r="E125" s="20" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125">
-        <v>40092</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="E125" s="19" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126">
+        <v>40092</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="E126" s="19" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127">
         <v>40095</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C127" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E126" s="19" t="s">
+      <c r="E127" s="19" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127">
-        <v>40094</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="E127" s="20" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A128">
+        <v>40094</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E128" s="20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129">
         <v>40098</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B129" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="C129" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="E128" s="20" t="s">
+      <c r="E129" s="20" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="13">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="13">
         <v>40140</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B130" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="C129" s="15" t="s">
+      <c r="C130" s="15" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130">
+    <row r="131" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131">
         <v>40123</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B131" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C130" s="7" t="s">
+      <c r="C131" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E130" s="19" t="s">
+      <c r="E131" s="19" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131">
-        <v>40032</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E131" s="19" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132">
+        <v>40032</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E132" s="19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133">
         <v>40013</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B133" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C132" s="7" t="s">
+      <c r="C133" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E132" s="19" t="s">
+      <c r="E133" s="19" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134">
         <v>40001</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B134" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C134" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E133" s="19" t="s">
+      <c r="E134" s="19" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134">
+    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135">
         <v>40036</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B135" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C135" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E134" s="19" t="s">
+      <c r="E135" s="19" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135">
+    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136">
         <v>40104</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B136" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C136" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E135" s="19" t="s">
+      <c r="E136" s="19" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136">
+    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137">
         <v>40105</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B137" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C137" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E136" s="19" t="s">
+      <c r="E137" s="19" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137">
+    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138">
         <v>40097</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B138" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C137" s="7" t="s">
+      <c r="C138" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="E137" s="19" t="s">
+      <c r="E138" s="19" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138">
-        <v>40019</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="E138" s="19" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139">
+        <v>40019</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E139" s="19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140">
         <v>40128</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="B140" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="C139" s="7" t="s">
+      <c r="C140" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D140" t="s">
         <v>313</v>
       </c>
-      <c r="E139" s="19" t="s">
+      <c r="E140" s="19" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="13">
+    <row r="141" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="13">
         <v>40077</v>
       </c>
-      <c r="B140" s="16" t="s">
+      <c r="B141" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="C141" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D140" s="13" t="s">
+      <c r="D141" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="E140" s="22" t="s">
+      <c r="E141" s="22" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141">
+    <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142">
         <v>40100</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B142" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C141" s="7" t="s">
+      <c r="C142" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="E141" s="19" t="s">
+      <c r="E142" s="19" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143">
         <v>40012</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="B143" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C143" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E142" s="19" t="s">
+      <c r="E143" s="19" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143">
+    <row r="144" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144">
         <v>40132</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B144" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C144" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="E143" s="19" t="s">
+      <c r="E144" s="19" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144">
+    <row r="145" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145">
         <v>40133</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C144" s="7" t="s">
+      <c r="C145" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="E144" s="19" t="s">
+      <c r="E145" s="19" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146">
         <v>40135</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B146" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C145" s="7" t="s">
+      <c r="C146" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="E145" s="19" t="s">
+      <c r="E146" s="19" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146">
-        <v>40134</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="E146" s="19" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
+        <v>40134</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E147" s="19" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148">
         <v>40131</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C147" s="7" t="s">
+      <c r="C148" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="E147" s="19" t="s">
+      <c r="E148" s="19" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148">
+    <row r="149" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149">
         <v>40137</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B149" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C148" s="7" t="s">
+      <c r="C149" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="E148" s="20" t="s">
+      <c r="E149" s="20" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149">
-        <v>40136</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="E149" s="19" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
-        <v>40138</v>
+        <v>40136</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E150" s="19" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151">
+        <v>40138</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E151" s="19" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152">
         <v>40141</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B152" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C151" s="7" t="s">
+      <c r="C152" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="E151" s="20" t="s">
+      <c r="E152" s="20" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A152">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153">
         <v>40129</v>
       </c>
-      <c r="B152" s="11" t="s">
+      <c r="B153" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="C152" s="7" t="s">
+      <c r="C153" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D153" t="s">
         <v>313</v>
       </c>
-      <c r="E152" s="19" t="s">
+      <c r="E153" s="19" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B153" s="16" t="s">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B154" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="C153" s="7" t="s">
+      <c r="C154" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="E153" s="19" t="s">
+      <c r="E154" s="19" t="s">
         <v>368</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nebulizer, pressurized, liquide rectale, anneau à libération lente
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie\Documents\GitHub\formulary\Working QA Team Folders\Guidance documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\OneDrive\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Guidance documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C703FB5-081C-4EFB-86FA-DA21E4506950}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB397A77-20E3-41B1-BE08-6749D670CC5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="501">
   <si>
     <t>NTP Formal Name Dose form</t>
   </si>
@@ -72,9 +72,6 @@
     <t>cutaneous foam</t>
   </si>
   <si>
-    <t>Liquid, usually multidose preparation, usually presented in a pressurised container equipped with an applicator suitable for delivery of a foam consisting of large volumes of gas dispersed in a liquid containing active substance(s). Cutaneous foams are intended for cutaneous use</t>
-  </si>
-  <si>
     <t>cutaneous gel</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>cutaneous spray</t>
-  </si>
-  <si>
-    <t>Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) in a pressurised container with a spray valve or in a container equipped with a spray pump, intended for cutaneous use</t>
   </si>
   <si>
     <t>Not present in EDQM explicitly (more granular concepts present).  "Cutaneous spray" is the patient-friendly term in EDQM</t>
@@ -296,9 +290,6 @@
     <t>inhalation solution</t>
   </si>
   <si>
-    <t>Liquid, usually multidose preparation consisting of a solution intended for inhalation use. The preparation is presented in a non-pressurised container fitted with a metering dose mechanism. 'Nebuliser solution' and 'Pressurised inhalation, solution' are excluded</t>
-  </si>
-  <si>
     <t>inhalation vapour (liquid)</t>
   </si>
   <si>
@@ -448,18 +439,6 @@
     <t>Solid single-dose preparation, usually rod-shaped or conical, intended for nasal use to obtain a local effect</t>
   </si>
   <si>
-    <t>nebuliser solution</t>
-  </si>
-  <si>
-    <t>Liquid preparation consisting of a solution intended for inhalation use. The solution is converted into an aerosol by a continuously operating nebuliser or a metered-dose nebuliser</t>
-  </si>
-  <si>
-    <t>nebuliser suspension</t>
-  </si>
-  <si>
-    <t>Liquid preparation consisting of a suspension intended for inhalation use. The suspension is converted into an aerosol by a continuously operating nebuliser or a metered-dose nebuliser</t>
-  </si>
-  <si>
     <t>ophthalmic cream</t>
   </si>
   <si>
@@ -599,9 +578,6 @@
   </si>
   <si>
     <t>oromucosal spray</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) intended for oromucosal use. It is administered by spraying into the oral cavity or onto a specific part of the oral cavity or the throat. It is presented in a container with a spray pump or in a pressurised container with or without a metering valve. Sublingual sprays are excluded</t>
   </si>
   <si>
     <t xml:space="preserve">"Oromucosal spray" is a deprecated concept in EDQM (more granular concepts present).  </t>
@@ -696,12 +672,6 @@
     <t>Solid preparation consisting of one or more powders, including freeze-dried powders, intended to be dispersed in the specified liquid to obtain an intravesical suspension</t>
   </si>
   <si>
-    <t>powder for nebuliser solution</t>
-  </si>
-  <si>
-    <t>Solid preparation consisting of one or more powders, including freeze-dried powders, intended to be dissolved in the specified liquid to obtain a nebuliser solution</t>
-  </si>
-  <si>
     <t>powder for ophthalmic drops</t>
   </si>
   <si>
@@ -770,12 +740,6 @@
     <t xml:space="preserve"> Solid sterile preparation consisting of one or more powders, including freeze-dried powders, intended to be dispersed in the specified liquid to obtain a suspension for injection</t>
   </si>
   <si>
-    <t>pressurised inhalation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liquid, usually multidose preparation consisting of a solution, emulsion or suspension intended for inhalation use. The preparation is presented in a pressurised container usually fitted with a metering dose valve. </t>
-  </si>
-  <si>
     <t>Liquid sterile single-dose or multidose preparation intended for ocular use. The active substance is released over an extended period of time</t>
   </si>
   <si>
@@ -809,9 +773,6 @@
     <t>rectal foam</t>
   </si>
   <si>
-    <t>Liquid preparation, usually presented to in a pressurised container provided with an applicator suitable for delivery to the rectum of foam containing large volumes of gas dispersed in a liquid containing the active substance.  Rectal foams are intended for local effect.</t>
-  </si>
-  <si>
     <t>rectal gel</t>
   </si>
   <si>
@@ -873,9 +834,6 @@
   </si>
   <si>
     <t>sublingual spray</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) intended for sublingual use. Sublingual sprays are usually presented in pressurised containers with a metering valve</t>
   </si>
   <si>
     <t>sublingual tablet</t>
@@ -1307,9 +1265,6 @@
     <t>liquide oral</t>
   </si>
   <si>
-    <t>liquide rectale</t>
-  </si>
-  <si>
     <t>mousse rectale</t>
   </si>
   <si>
@@ -1531,9 +1486,6 @@
   </si>
   <si>
     <t>cutaneous spray powder</t>
-  </si>
-  <si>
-    <t>Solid, usually multidose preparation presented in a pressurised container with a spray valve or in a container equipped with a spray pump.  The spray is intended for cutaneous use</t>
   </si>
   <si>
     <t>EDQM</t>
@@ -1639,9 +1591,6 @@
     <t>injectable foam</t>
   </si>
   <si>
-    <t>Liquid, usually multidose preparation, usually presented in a pressurised container or with pressurising equipment to enable delivery of a foam consisting of large volumes of gas dispersed in a liquid containing active substance(s) to be administered by injection.</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOT an EDQM term; added for polidocanol injectable foam (VARITHENA). </t>
   </si>
   <si>
@@ -1682,6 +1631,60 @@
   </si>
   <si>
     <t>Note that products that use this dose form should have a "per actuation" strength; is mostly used for 'mist' inhalers</t>
+  </si>
+  <si>
+    <t>nebulizer solution</t>
+  </si>
+  <si>
+    <t>nebulizer suspension</t>
+  </si>
+  <si>
+    <t>powder for nebulizer solution</t>
+  </si>
+  <si>
+    <t>Liquid preparation consisting of a solution intended for inhalation use. The solution is converted into an aerosol by a continuously operating nebulizer or a metered-dose nebulizer</t>
+  </si>
+  <si>
+    <t>Liquid preparation consisting of a suspension intended for inhalation use. The suspension is converted into an aerosol by a continuously operating nebulizer or a metered-dose nebulizer</t>
+  </si>
+  <si>
+    <t>Solid preparation consisting of one or more powders, including freeze-dried powders, intended to be dissolved in the specified liquid to obtain a nebulizer solution</t>
+  </si>
+  <si>
+    <t>Liquid, usually multidose preparation, usually presented in a pressurized container equipped with an applicator suitable for delivery of a foam consisting of large volumes of gas dispersed in a liquid containing active substance(s). Cutaneous foams are intended for cutaneous use</t>
+  </si>
+  <si>
+    <t>Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) in a pressurized container with a spray valve or in a container equipped with a spray pump, intended for cutaneous use</t>
+  </si>
+  <si>
+    <t>Solid, usually multidose preparation presented in a pressurized container with a spray valve or in a container equipped with a spray pump.  The spray is intended for cutaneous use</t>
+  </si>
+  <si>
+    <t>Liquid, usually multidose preparation consisting of a solution intended for inhalation use. The preparation is presented in a non-pressurized container fitted with a metering dose mechanism. 'nebulizer solution' and 'pressurized inhalation, solution' are excluded</t>
+  </si>
+  <si>
+    <t>Liquid, usually multidose preparation, usually presented in a pressurized container or with pressurising equipment to enable delivery of a foam consisting of large volumes of gas dispersed in a liquid containing active substance(s) to be administered by injection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) intended for oromucosal use. It is administered by spraying into the oral cavity or onto a specific part of the oral cavity or the throat. It is presented in a container with a spray pump or in a pressurized container with or without a metering valve. Sublingual sprays are excluded</t>
+  </si>
+  <si>
+    <t>pressurized inhalation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liquid, usually multidose preparation consisting of a solution, emulsion or suspension intended for inhalation use. The preparation is presented in a pressurized container usually fitted with a metering dose valve. </t>
+  </si>
+  <si>
+    <t>Liquid preparation, usually presented to in a pressurized container provided with an applicator suitable for delivery to the rectum of foam containing large volumes of gas dispersed in a liquid containing the active substance.  Rectal foams are intended for local effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liquid, usually multidose preparation consisting of a preparation (solution/suspension/emulsion) intended for sublingual use. Sublingual sprays are usually presented in pressurized containers with a metering valve</t>
+  </si>
+  <si>
+    <t>liquide rectal</t>
+  </si>
+  <si>
+    <t>anneau à libération lente</t>
   </si>
 </sst>
 </file>
@@ -2148,23 +2151,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="103.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="103.578125" customWidth="1"/>
+    <col min="4" max="4" width="27.83984375" customWidth="1"/>
+    <col min="5" max="5" width="54.578125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2176,10 +2179,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>40007</v>
       </c>
@@ -2190,24 +2193,24 @@
         <v>4</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>40146</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>40079</v>
       </c>
@@ -2221,10 +2224,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>40108</v>
       </c>
@@ -2238,10 +2241,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>40111</v>
       </c>
@@ -2252,10 +2255,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>40107</v>
       </c>
@@ -2263,2176 +2266,2179 @@
         <v>13</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>489</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>40112</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>40113</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="E9" s="20" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>40116</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="20" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>40118</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="E11" s="20" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>40119</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="E12" s="20" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>40121</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="E13" s="20" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>40124</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="E14" s="20" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>40106</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="E15" s="20" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>455</v>
+        <v>491</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>40126</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="20" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>40127</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>40010</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>40011</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>40084</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="13">
         <v>40109</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="21" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>40082</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>40142</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25">
         <v>40015</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26">
         <v>40033</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>40037</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="E27" s="20" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>40004</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>40048</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="E29" s="20" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>40071</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>40081</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>40069</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>40068</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>40101</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>40025</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>40022</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="19" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>40027</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>76</v>
+        <v>492</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>40024</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="3" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>40034</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>40038</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>40041</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>40042</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>40035</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="13">
         <v>40006</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>40115</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="13">
         <v>40114</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>40073</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>40130</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>40023</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>40061</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>40080</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>40003</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="16" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>40046</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>40043</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>40044</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>40045</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>40030</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>40029</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>40047</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>40031</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>122</v>
+        <v>483</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>123</v>
+        <v>486</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>40028</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>124</v>
+        <v>484</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>125</v>
+        <v>487</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>40057</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>40050</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>40051</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D66" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>40052</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>40053</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D68" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>40056</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>40058</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>40059</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="D71" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>40060</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>40063</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>40144</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>40145</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="20" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>40065</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>40067</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>40072</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>40075</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>40074</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>40064</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>40070</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <v>40078</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" s="3" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="19" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>40066</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>40076</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>40002</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>40009</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <v>40008</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>40005</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>173</v>
+        <v>494</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="3" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="23" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <v>40089</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D92" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E92" s="19" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
         <v>40086</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>40087</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D94" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E94" s="19" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
         <v>40088</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D95" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <v>40090</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D96" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E96" s="19" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <v>40117</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="E97" s="19" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <v>40102</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <v>40139</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E99" s="19" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>40120</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <v>40014</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E101" s="20" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <v>40122</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <v>40040</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <v>40026</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>200</v>
+        <v>485</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>201</v>
+        <v>488</v>
       </c>
       <c r="E104" s="19" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
         <v>40054</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E105" s="19" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
         <v>40049</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="12"/>
       <c r="B107" s="3" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
         <v>40085</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E108" s="19" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" s="3" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
         <v>40018</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E110" s="19" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
         <v>40096</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E111" s="19" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
         <v>40017</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E112" s="19" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="12"/>
       <c r="B113" s="3" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="E113" s="19" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A114">
         <v>40039</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
         <v>40016</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116">
         <v>40021</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>220</v>
+        <v>495</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>221</v>
+        <v>496</v>
       </c>
       <c r="E116" s="19" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117">
         <v>40055</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E117" s="19" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
         <v>40062</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E118" s="19" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A119">
         <v>40083</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E119" s="19" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A120">
         <v>40103</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E120" s="20" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" s="3" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="20" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A122">
         <v>40020</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="E122" s="20" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123">
         <v>40099</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E123" s="19" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A124">
         <v>40091</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>233</v>
+        <v>497</v>
       </c>
       <c r="E124" s="20" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A125">
         <v>40093</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126">
         <v>40092</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="E126" s="19" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127">
         <v>40095</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E127" s="19" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A128">
         <v>40094</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="E128" s="20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A129">
         <v>40098</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E129" s="20" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="13">
         <v>40140</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="E130" s="19" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A131">
         <v>40123</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="E131" s="19" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132">
         <v>40032</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="E132" s="19" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A133">
         <v>40013</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E133" s="19" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134">
         <v>40001</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="E134" s="19" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A135">
         <v>40036</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="E135" s="19" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A136">
         <v>40104</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>255</v>
+        <v>498</v>
       </c>
       <c r="E136" s="19" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A137">
         <v>40105</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="E137" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A138">
         <v>40097</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="E138" s="19" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139">
         <v>40019</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="E139" s="19" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A140">
         <v>40128</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="D140" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="E140" s="19" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="13">
         <v>40077</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D141" s="13" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="E141" s="22" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A142">
         <v>40100</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="E142" s="19" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A143">
         <v>40012</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="E143" s="19" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A144">
         <v>40132</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="E144" s="19" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A145">
         <v>40133</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="E145" s="19" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A146">
         <v>40135</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="E146" s="19" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
         <v>40134</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="E147" s="19" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148">
         <v>40131</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="E148" s="19" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A149">
         <v>40137</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="E149" s="20" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
         <v>40136</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="E150" s="19" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151">
         <v>40138</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="E151" s="19" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152">
         <v>40141</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="E152" s="20" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A153">
         <v>40129</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="D153" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="E153" s="19" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B154" s="16" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="E154" s="19" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NTP DF concepts: add code for buccal/sublingual film
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
+++ b/Working QA Team Folders/Guidance documents/CCDD NTP Dosage form concepts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BAJOVAIS\Documents\GitHub\formulary\Working QA Team Folders\Guidance documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\HC\HPFB\TPD\TPD\X_REFERENCE\OSIP\DIN\DIN Mgmt Div\CCDD Unit\Guidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2069,13 +2069,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF5050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2121,7 +2121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2131,7 +2131,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2176,9 +2176,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2233,12 +2230,20 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2516,8 +2521,8 @@
   <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,6 +2589,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>40154</v>
+      </c>
       <c r="B4" s="21" t="s">
         <v>542</v>
       </c>
@@ -2722,7 +2730,7 @@
       <c r="D11" s="22">
         <v>10512000</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="43" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="24" t="s">
@@ -2830,7 +2838,7 @@
       <c r="D17" s="22">
         <v>15090</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="43" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="24" t="s">
@@ -2939,16 +2947,16 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="A24" s="42">
         <v>40153</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>534</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="25" t="s">
         <v>535</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="26">
         <v>50077000</v>
       </c>
       <c r="F24" s="24" t="s">
@@ -2956,18 +2964,18 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="A25" s="27">
         <v>40109</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31" t="s">
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="30" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3008,7 +3016,7 @@
       <c r="A28" s="17">
         <v>40015</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="31" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="19" t="s">
@@ -3023,7 +3031,7 @@
       <c r="A29" s="17">
         <v>40033</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -3045,7 +3053,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="19"/>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="43" t="s">
         <v>53</v>
       </c>
       <c r="F30" s="24" t="s">
@@ -3071,13 +3079,13 @@
       <c r="A32" s="17">
         <v>40048</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="35"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="19" t="s">
         <v>58</v>
       </c>
@@ -3092,10 +3100,10 @@
       <c r="B33" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="34" t="s">
         <v>497</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="34">
         <v>50026000</v>
       </c>
       <c r="F33" s="24" t="s">
@@ -3106,7 +3114,7 @@
       <c r="A34" s="17">
         <v>40081</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="19" t="s">
@@ -3189,11 +3197,11 @@
       <c r="B39" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="37"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="20" t="s">
         <v>375</v>
       </c>
@@ -3253,10 +3261,10 @@
       <c r="B43" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="36"/>
+      <c r="D43" s="35"/>
       <c r="F43" s="24" t="s">
         <v>378</v>
       </c>
@@ -3325,16 +3333,16 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+      <c r="A48" s="27">
         <v>40006</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="D48" s="29"/>
+      <c r="D48" s="28"/>
     </row>
     <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
@@ -3355,17 +3363,17 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="28">
+      <c r="A50" s="27">
         <v>40114</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29" t="s">
+      <c r="D50" s="28"/>
+      <c r="E50" s="28" t="s">
         <v>310</v>
       </c>
       <c r="F50" s="20" t="s">
@@ -3472,14 +3480,14 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="38"/>
+      <c r="A57" s="37"/>
       <c r="B57" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="28" t="s">
         <v>467</v>
       </c>
-      <c r="D57" s="29"/>
+      <c r="D57" s="28"/>
       <c r="E57" s="19" t="s">
         <v>468</v>
       </c>
@@ -3613,7 +3621,7 @@
       <c r="E65" s="19" t="s">
         <v>538</v>
       </c>
-      <c r="F65" s="39" t="s">
+      <c r="F65" s="38" t="s">
         <v>539</v>
       </c>
     </row>
@@ -3789,7 +3797,7 @@
       <c r="A76" s="17">
         <v>40060</v>
       </c>
-      <c r="B76" s="34" t="s">
+      <c r="B76" s="33" t="s">
         <v>130</v>
       </c>
       <c r="C76" s="19" t="s">
@@ -3825,7 +3833,7 @@
       <c r="A78" s="17">
         <v>40144</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="39" t="s">
         <v>431</v>
       </c>
       <c r="C78" s="19" t="s">
@@ -3841,7 +3849,7 @@
       <c r="A79" s="17">
         <v>40145</v>
       </c>
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="39" t="s">
         <v>432</v>
       </c>
       <c r="C79" s="19" t="s">
@@ -4029,10 +4037,10 @@
       <c r="B91" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C91" s="36" t="s">
+      <c r="C91" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="D91" s="36"/>
+      <c r="D91" s="35"/>
       <c r="F91" s="20" t="s">
         <v>411</v>
       </c>
@@ -4083,7 +4091,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="38"/>
+      <c r="A95" s="37"/>
       <c r="B95" s="21" t="s">
         <v>473</v>
       </c>
@@ -4092,7 +4100,7 @@
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="19"/>
-      <c r="F95" s="39" t="s">
+      <c r="F95" s="38" t="s">
         <v>475</v>
       </c>
     </row>
@@ -4190,7 +4198,7 @@
       <c r="A101" s="17">
         <v>40117</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="39" t="s">
         <v>280</v>
       </c>
       <c r="C101" s="19" t="s">
@@ -4238,7 +4246,7 @@
       <c r="A104" s="17">
         <v>40120</v>
       </c>
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="39" t="s">
         <v>279</v>
       </c>
       <c r="C104" s="19" t="s">
@@ -4346,7 +4354,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A111" s="38"/>
+      <c r="A111" s="37"/>
       <c r="B111" s="21" t="s">
         <v>191</v>
       </c>
@@ -4434,7 +4442,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="38"/>
+      <c r="A117" s="37"/>
       <c r="B117" s="21" t="s">
         <v>437</v>
       </c>
@@ -4483,7 +4491,7 @@
       <c r="A120" s="17">
         <v>40021</v>
       </c>
-      <c r="B120" s="34" t="s">
+      <c r="B120" s="33" t="s">
         <v>489</v>
       </c>
       <c r="C120" s="19" t="s">
@@ -4550,7 +4558,7 @@
         <v>209</v>
       </c>
       <c r="D124" s="19"/>
-      <c r="E124" s="36" t="s">
+      <c r="E124" s="35" t="s">
         <v>210</v>
       </c>
       <c r="F124" s="24" t="s">
@@ -4568,7 +4576,7 @@
         <v>424</v>
       </c>
       <c r="D125" s="19"/>
-      <c r="E125" s="36"/>
+      <c r="E125" s="35"/>
       <c r="F125" s="24" t="s">
         <v>425</v>
       </c>
@@ -4698,16 +4706,16 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="28">
+      <c r="A134" s="27">
         <v>40140</v>
       </c>
-      <c r="B134" s="41" t="s">
+      <c r="B134" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="C134" s="29" t="s">
+      <c r="C134" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="D134" s="29"/>
+      <c r="D134" s="28"/>
       <c r="F134" s="20" t="s">
         <v>494</v>
       </c>
@@ -4791,7 +4799,7 @@
       <c r="A140" s="17">
         <v>40151</v>
       </c>
-      <c r="B140" s="40" t="s">
+      <c r="B140" s="39" t="s">
         <v>526</v>
       </c>
       <c r="C140" s="19" t="s">
@@ -4868,7 +4876,7 @@
       <c r="A145" s="17">
         <v>40128</v>
       </c>
-      <c r="B145" s="40" t="s">
+      <c r="B145" s="39" t="s">
         <v>282</v>
       </c>
       <c r="C145" s="19" t="s">
@@ -4883,20 +4891,20 @@
       </c>
     </row>
     <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A146" s="28">
+      <c r="A146" s="27">
         <v>40077</v>
       </c>
       <c r="B146" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="C146" s="29" t="s">
+      <c r="C146" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="D146" s="29"/>
-      <c r="E146" s="28" t="s">
+      <c r="D146" s="28"/>
+      <c r="E146" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="F146" s="42" t="s">
+      <c r="F146" s="41" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4964,7 +4972,7 @@
       <c r="A151" s="17">
         <v>40146</v>
       </c>
-      <c r="B151" s="40" t="s">
+      <c r="B151" s="39" t="s">
         <v>528</v>
       </c>
       <c r="C151" s="19" t="s">
@@ -5086,7 +5094,7 @@
       <c r="A159" s="17">
         <v>40129</v>
       </c>
-      <c r="B159" s="40" t="s">
+      <c r="B159" s="39" t="s">
         <v>283</v>
       </c>
       <c r="C159" s="19" t="s">

</xml_diff>